<commit_message>
Schedule and Grading Sheet Updated
</commit_message>
<xml_diff>
--- a/Milestone_Grading_Sheet.xlsx
+++ b/Milestone_Grading_Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\traeg\Documents\CS461\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\traeg\Documents\CS461\404notfoundproj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{AF935ADE-A56B-47EB-9D80-A0641943CBFC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB693073-3996-4BEC-9085-123D1265FD39}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Milestone_1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="Milestone_4" sheetId="4" r:id="rId4"/>
     <sheet name="Milestone_5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="45">
   <si>
     <t>CS 461: Software Engineering II</t>
   </si>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20">
     <font>
       <sz val="11"/>
@@ -427,7 +427,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -473,35 +473,38 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="18">
-    <cellStyle name="Accent" xfId="7"/>
-    <cellStyle name="Accent 1" xfId="8"/>
-    <cellStyle name="Accent 2" xfId="9"/>
-    <cellStyle name="Accent 3" xfId="10"/>
+    <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent 1" xfId="8" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent 3" xfId="10" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Bad" xfId="4" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Error" xfId="11"/>
-    <cellStyle name="Footnote" xfId="12"/>
+    <cellStyle name="Error" xfId="11" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Footnote" xfId="12" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Good" xfId="3" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading" xfId="13"/>
+    <cellStyle name="Heading" xfId="13" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="14"/>
+    <cellStyle name="Hyperlink" xfId="14" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Neutral" xfId="5" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Note" xfId="6" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Status" xfId="15"/>
-    <cellStyle name="Text" xfId="16"/>
-    <cellStyle name="Warning" xfId="17"/>
+    <cellStyle name="Status" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Text" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Warning" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -812,10 +815,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -830,12 +833,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
       <c r="A2" s="1" t="s">
@@ -1009,11 +1012,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1027,12 +1030,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
       <c r="A2" s="1" t="s">
@@ -1046,7 +1049,9 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="15.6">
       <c r="A4" s="1" t="s">
@@ -1064,28 +1069,37 @@
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="21.6" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="D7" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="B7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:4" ht="21.6" customHeight="1">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="8" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="21.6" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="16.2" thickBot="1">
       <c r="A11" s="10" t="s">
@@ -1102,68 +1116,68 @@
       </c>
     </row>
     <row r="12" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1" thickTop="1">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="19"/>
+      <c r="D12" s="18"/>
     </row>
     <row r="13" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="19"/>
+      <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="19"/>
+      <c r="D14" s="18"/>
     </row>
     <row r="15" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="19"/>
+      <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" s="18"/>
     </row>
     <row r="17" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="19"/>
+      <c r="D17" s="18"/>
     </row>
     <row r="18" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="19"/>
+      <c r="D18" s="18"/>
     </row>
     <row r="19" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="19"/>
+      <c r="D19" s="18"/>
     </row>
     <row r="20" spans="1:4" s="14" customFormat="1" ht="35.549999999999997" customHeight="1">
       <c r="A20" s="15"/>
@@ -1177,8 +1191,9 @@
     <row r="24" spans="1:4" s="14" customFormat="1"/>
     <row r="25" spans="1:4" s="14" customFormat="1"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="D6:D7"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.4" bottom="0.4" header="0" footer="0"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1190,7 +1205,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1206,12 +1221,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
       <c r="A2" s="1" t="s">
@@ -1281,68 +1296,68 @@
       </c>
     </row>
     <row r="12" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1" thickTop="1">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="19"/>
+      <c r="D12" s="18"/>
     </row>
     <row r="13" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="19"/>
+      <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="19"/>
+      <c r="D14" s="18"/>
     </row>
     <row r="15" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="19"/>
+      <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" s="18"/>
     </row>
     <row r="17" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="19"/>
+      <c r="D17" s="18"/>
     </row>
     <row r="18" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="19"/>
+      <c r="D18" s="18"/>
     </row>
     <row r="19" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="19"/>
+      <c r="D19" s="18"/>
     </row>
     <row r="20" spans="1:4" s="14" customFormat="1" ht="35.549999999999997" customHeight="1">
       <c r="A20" s="15"/>
@@ -1369,7 +1384,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1385,12 +1400,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
       <c r="A2" s="1" t="s">
@@ -1460,52 +1475,52 @@
       </c>
     </row>
     <row r="12" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1" thickTop="1">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="12"/>
-      <c r="D12" s="19"/>
+      <c r="D12" s="18"/>
     </row>
     <row r="13" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="12"/>
-      <c r="D13" s="19"/>
+      <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="12"/>
-      <c r="D14" s="19"/>
+      <c r="D14" s="18"/>
     </row>
     <row r="15" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="12"/>
-      <c r="D15" s="19"/>
+      <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="12"/>
-      <c r="D16" s="19"/>
+      <c r="D16" s="18"/>
     </row>
     <row r="17" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="12"/>
-      <c r="D17" s="19"/>
+      <c r="D17" s="18"/>
     </row>
     <row r="18" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="12"/>
-      <c r="D18" s="19"/>
+      <c r="D18" s="18"/>
     </row>
     <row r="19" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="12"/>
-      <c r="D19" s="19"/>
+      <c r="D19" s="18"/>
     </row>
     <row r="20" spans="1:4" s="14" customFormat="1" ht="35.549999999999997" customHeight="1">
       <c r="A20" s="15"/>
@@ -1532,7 +1547,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1548,12 +1563,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
       <c r="A2" s="1" t="s">
@@ -1623,52 +1638,52 @@
       </c>
     </row>
     <row r="12" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1" thickTop="1">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="12"/>
-      <c r="D12" s="19"/>
+      <c r="D12" s="18"/>
     </row>
     <row r="13" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="12"/>
-      <c r="D13" s="19"/>
+      <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="12"/>
-      <c r="D14" s="19"/>
+      <c r="D14" s="18"/>
     </row>
     <row r="15" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="12"/>
-      <c r="D15" s="19"/>
+      <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="12"/>
-      <c r="D16" s="19"/>
+      <c r="D16" s="18"/>
     </row>
     <row r="17" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="12"/>
-      <c r="D17" s="19"/>
+      <c r="D17" s="18"/>
     </row>
     <row r="18" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="12"/>
-      <c r="D18" s="19"/>
+      <c r="D18" s="18"/>
     </row>
     <row r="19" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="12"/>
-      <c r="D19" s="19"/>
+      <c r="D19" s="18"/>
     </row>
     <row r="20" spans="1:4" s="14" customFormat="1" ht="35.549999999999997" customHeight="1">
       <c r="A20" s="15"/>

</xml_diff>

<commit_message>
Added MS2 Names to Assignments
</commit_message>
<xml_diff>
--- a/Milestone_Grading_Sheet.xlsx
+++ b/Milestone_Grading_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\traeg\Documents\CS461\404notfoundproj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C81DCD-7E2A-462D-AD4D-405BEB7F8143}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652350A2-5681-42DF-B7C2-AD676F064585}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Milestone_1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="49">
   <si>
     <t>CS 461: Software Engineering II</t>
   </si>
@@ -1027,7 +1027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -1236,7 +1236,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
@@ -1268,7 +1270,9 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="15.6">
       <c r="A4" s="1" t="s">
@@ -1286,28 +1290,37 @@
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="21.6" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="D7" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="B7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:4" ht="21.6" customHeight="1">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="8" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="21.6" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="16.2" thickBot="1">
       <c r="A11" s="10" t="s">
@@ -1331,7 +1344,7 @@
       </c>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
+    <row r="13" spans="1:4" s="14" customFormat="1" ht="63" customHeight="1">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="12" t="s">
@@ -1399,8 +1412,9 @@
     <row r="24" spans="1:4" s="14" customFormat="1"/>
     <row r="25" spans="1:4" s="14" customFormat="1"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="D6:D7"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.4" bottom="0.4" header="0" footer="0"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1415,7 +1429,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>

</xml_diff>

<commit_message>
Edited Grading Sheet for MS3
</commit_message>
<xml_diff>
--- a/Milestone_Grading_Sheet.xlsx
+++ b/Milestone_Grading_Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\traeg\Documents\CS461\404notfoundproj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652350A2-5681-42DF-B7C2-AD676F064585}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90474D8C-FABA-432E-BB8B-CA0A5D3664CA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="54">
   <si>
     <t>CS 461: Software Engineering II</t>
   </si>
@@ -171,6 +171,21 @@
   </si>
   <si>
     <t>Joe/Megan</t>
+  </si>
+  <si>
+    <t>Joe/Team</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Mind Map - Joe</t>
+  </si>
+  <si>
+    <t>Vision Statement/Description - Shay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Needs and Features/Requirements - </t>
   </si>
 </sst>
 </file>
@@ -338,7 +353,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -418,6 +433,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -439,7 +484,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -489,6 +534,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -830,7 +881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -845,12 +896,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
       <c r="A2" s="1" t="s">
@@ -1042,12 +1093,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
       <c r="A2" s="1" t="s">
@@ -1084,7 +1135,7 @@
       <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="22" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1095,7 +1146,7 @@
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:4" ht="21.6" customHeight="1">
       <c r="A8" s="7" t="s">
@@ -1236,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1251,12 +1302,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
       <c r="A2" s="1" t="s">
@@ -1293,7 +1344,7 @@
       <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="22" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1304,7 +1355,7 @@
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:4" ht="21.6" customHeight="1">
       <c r="A8" s="7" t="s">
@@ -1338,67 +1389,83 @@
     </row>
     <row r="12" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1" thickTop="1">
       <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
+      <c r="B12" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="C12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="18"/>
+      <c r="D12" s="19"/>
     </row>
     <row r="13" spans="1:4" s="14" customFormat="1" ht="63" customHeight="1">
       <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
+      <c r="B13" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="C13" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="18"/>
+      <c r="D13" s="20"/>
     </row>
     <row r="14" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
       <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
+      <c r="B14" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="C14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="18"/>
+      <c r="D14" s="20"/>
     </row>
     <row r="15" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
       <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
+      <c r="B15" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="C15" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="20"/>
     </row>
     <row r="16" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
       <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
+      <c r="B16" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="C16" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="18"/>
+      <c r="D16" s="20"/>
     </row>
     <row r="17" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
       <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
+      <c r="B17" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="C17" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="18"/>
+      <c r="D17" s="20"/>
     </row>
     <row r="18" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
       <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
+      <c r="B18" s="11" t="s">
+        <v>52</v>
+      </c>
       <c r="C18" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="18"/>
+      <c r="D18" s="20"/>
     </row>
     <row r="19" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
       <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
+      <c r="B19" s="11" t="s">
+        <v>53</v>
+      </c>
       <c r="C19" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="18"/>
+      <c r="D19" s="20"/>
     </row>
     <row r="20" spans="1:4" s="14" customFormat="1" ht="35.549999999999997" customHeight="1">
       <c r="A20" s="15"/>
@@ -1444,12 +1511,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
       <c r="A2" s="1" t="s">
@@ -1607,12 +1674,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
Fixed Navbar and Ran CodeMaid Cleanup
</commit_message>
<xml_diff>
--- a/Milestone_Grading_Sheet.xlsx
+++ b/Milestone_Grading_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\traeg\Documents\CS461\404notfoundproj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90474D8C-FABA-432E-BB8B-CA0A5D3664CA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5246F1-87FB-4F5C-BD83-4ADB8DFFAFD1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -185,7 +185,7 @@
     <t>Vision Statement/Description - Shay</t>
   </si>
   <si>
-    <t xml:space="preserve">Needs and Features/Requirements - </t>
+    <t>Needs and Features/Requirements - Joe</t>
   </si>
 </sst>
 </file>
@@ -1287,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>

<commit_message>
Added MS4 to the Grading Sheet
</commit_message>
<xml_diff>
--- a/Milestone_Grading_Sheet.xlsx
+++ b/Milestone_Grading_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\traeg\Documents\CS461\404notfoundproj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5246F1-87FB-4F5C-BD83-4ADB8DFFAFD1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1963170-056C-4975-B3E7-BE4BDC642B0D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Milestone_1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="65">
   <si>
     <t>CS 461: Software Engineering II</t>
   </si>
@@ -186,13 +186,46 @@
   </si>
   <si>
     <t>Needs and Features/Requirements - Joe</t>
+  </si>
+  <si>
+    <t>Class Project: Sprint 2 planning</t>
+  </si>
+  <si>
+    <t>Class Project: Sprint 2 construction</t>
+  </si>
+  <si>
+    <t>Team Project Inception</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> / 40</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Team (Via Pivotal Tracker)</t>
+  </si>
+  <si>
+    <t>Joe - Needs and Features / User Stories / Requirements / NFR</t>
+  </si>
+  <si>
+    <t>Shay/Megan - WireFrame</t>
+  </si>
+  <si>
+    <t>Sodara - Timeline / Release Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shay - ER Diagram / Architecture / Use Case </t>
+  </si>
+  <si>
+    <t>Megan - Identification of Risks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -300,6 +333,45 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Liberation Sans"/>
     </font>
   </fonts>
@@ -353,7 +425,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -463,8 +535,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
@@ -483,8 +609,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -548,26 +692,101 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="18"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="18" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="18" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="18" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="36">
     <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Accent 1" xfId="8" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent 1 2" xfId="26" xr:uid="{7A21DED8-FE52-4F5D-B9D1-630B4FDB0441}"/>
     <cellStyle name="Accent 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent 2 2" xfId="27" xr:uid="{4A781695-3251-420F-86C0-80229D25D1C9}"/>
     <cellStyle name="Accent 3" xfId="10" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Accent 3 2" xfId="28" xr:uid="{3A0F0430-41AC-4CA1-8026-A7786494601E}"/>
+    <cellStyle name="Accent 4" xfId="25" xr:uid="{58F7B6C0-0393-4237-B2FE-C9C8007491CD}"/>
     <cellStyle name="Bad" xfId="4" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Bad 2" xfId="22" xr:uid="{FC625AE0-002B-4554-AACE-24408616CC00}"/>
     <cellStyle name="Error" xfId="11" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Error 2" xfId="29" xr:uid="{0EB49467-795A-4AE3-8F8C-8231C46486CC}"/>
     <cellStyle name="Footnote" xfId="12" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Footnote 2" xfId="30" xr:uid="{7D13CC0E-580D-4A68-B334-976B546B137A}"/>
     <cellStyle name="Good" xfId="3" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Good 2" xfId="21" xr:uid="{13EDCF9E-9225-49D1-AEF0-DF84AE468E4D}"/>
     <cellStyle name="Heading" xfId="13" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 1 2" xfId="19" xr:uid="{5D78AACE-6C80-4AD3-9586-DAB2457AECC6}"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 2 2" xfId="20" xr:uid="{448207C1-EF39-4273-8F7A-0E48DC5B3B84}"/>
+    <cellStyle name="Heading 5" xfId="31" xr:uid="{05C7C849-83D6-45BD-B587-4C9A6BF4CA17}"/>
     <cellStyle name="Hyperlink" xfId="14" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="32" xr:uid="{ECFE451A-120C-4DB3-8239-8B8F2ADF4E0E}"/>
     <cellStyle name="Neutral" xfId="5" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutral 2" xfId="23" xr:uid="{B5AA2F2A-C1F2-4DD4-85E9-EF50B7A04180}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Normal 2" xfId="18" xr:uid="{E75F612D-9F88-4DB5-A927-0A580BBD126B}"/>
     <cellStyle name="Note" xfId="6" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Note 2" xfId="24" xr:uid="{3F7A8C25-15F9-47D2-82EA-36F6D33940F3}"/>
     <cellStyle name="Status" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Status 2" xfId="33" xr:uid="{B7F620DB-1218-44F8-9328-15DE2C210FAD}"/>
     <cellStyle name="Text" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Text 2" xfId="34" xr:uid="{1AA205D6-FF3D-4655-8908-D269FAF222D0}"/>
     <cellStyle name="Warning" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Warning 2" xfId="35" xr:uid="{A0D70F36-F53B-4B9C-812A-E275B63911E2}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1287,7 +1506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1496,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1511,133 +1730,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="25">
         <v>4</v>
       </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="1:4" ht="21.75" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
     </row>
     <row r="4" spans="1:4" ht="15.6">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
     </row>
     <row r="6" spans="1:4" ht="21.6" customHeight="1">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="38" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="21.6" customHeight="1">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="D7" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="B7" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" s="38"/>
     </row>
     <row r="8" spans="1:4" ht="21.6" customHeight="1">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
     </row>
     <row r="9" spans="1:4" ht="21.6" customHeight="1">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
     </row>
     <row r="11" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="32" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1" thickTop="1">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="18"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="39"/>
     </row>
     <row r="13" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="18"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="40"/>
     </row>
     <row r="14" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="18"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="40"/>
     </row>
     <row r="15" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="18"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="40"/>
     </row>
     <row r="16" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="18"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="33"/>
+      <c r="D16" s="40"/>
     </row>
     <row r="17" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="18"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="40"/>
     </row>
     <row r="18" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="18"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="33"/>
+      <c r="D18" s="40"/>
     </row>
     <row r="19" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="18"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="40"/>
     </row>
     <row r="20" spans="1:4" s="14" customFormat="1" ht="35.549999999999997" customHeight="1">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16" t="s">
-        <v>34</v>
-      </c>
+      <c r="A20" s="43"/>
+      <c r="B20" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
     </row>
     <row r="21" spans="1:4" s="14" customFormat="1"/>
     <row r="22" spans="1:4" s="14" customFormat="1"/>
@@ -1645,8 +1913,9 @@
     <row r="24" spans="1:4" s="14" customFormat="1"/>
     <row r="25" spans="1:4" s="14" customFormat="1"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="D6:D7"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.4" bottom="0.4" header="0" footer="0"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Readme, SQL Scripts, and Gradesheet updated
</commit_message>
<xml_diff>
--- a/Milestone_Grading_Sheet.xlsx
+++ b/Milestone_Grading_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\traeg\Documents\CS461\404notfoundproj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1963170-056C-4975-B3E7-BE4BDC642B0D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11AB6767-059F-46F7-9414-D58548149DB8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Milestone_1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="74">
   <si>
     <t>CS 461: Software Engineering II</t>
   </si>
@@ -219,6 +219,33 @@
   </si>
   <si>
     <t>Megan - Identification of Risks</t>
+  </si>
+  <si>
+    <t>Class Project Retrospective, results and summary</t>
+  </si>
+  <si>
+    <t>Class Project Continuous Deployment</t>
+  </si>
+  <si>
+    <t>Team Project Inception: last chance at defining things – markdown file is great.</t>
+  </si>
+  <si>
+    <t>Team Project Inception: Welcome page, guidelines, contributing to project, etc.</t>
+  </si>
+  <si>
+    <t>Team Project Sprint Planning: Pivotal Tracker set up correctly, Epics and Icebox are great, prioritized, top of Icebox (those going into Sprint 2) is well defined</t>
+  </si>
+  <si>
+    <t>Team Project Sprint I is well planned; correct number of stories/points and points are appropriate; stories are all well defined, have detailed description/specifications/requirements and tasks; are assigned</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> / 60</t>
+  </si>
+  <si>
+    <t>Shay - Full Markdown File</t>
+  </si>
+  <si>
+    <t>Joe - Pivotal Tracker | Descriptions - Team/Individualized</t>
   </si>
 </sst>
 </file>
@@ -628,7 +655,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -686,12 +713,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="18"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -725,29 +746,77 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="18" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="18" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="18"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="18" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="18" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="36">
@@ -1115,12 +1184,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
       <c r="A2" s="1" t="s">
@@ -1312,12 +1381,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
       <c r="A2" s="1" t="s">
@@ -1354,7 +1423,7 @@
       <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="41" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1365,7 +1434,7 @@
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="41"/>
     </row>
     <row r="8" spans="1:4" ht="21.6" customHeight="1">
       <c r="A8" s="7" t="s">
@@ -1521,12 +1590,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
       <c r="A2" s="1" t="s">
@@ -1563,7 +1632,7 @@
       <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="41" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1574,7 +1643,7 @@
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="41"/>
     </row>
     <row r="8" spans="1:4" ht="21.6" customHeight="1">
       <c r="A8" s="7" t="s">
@@ -1715,7 +1784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1730,182 +1799,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="23">
         <v>4</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
     </row>
     <row r="3" spans="1:4" ht="21.75" customHeight="1">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
     </row>
     <row r="4" spans="1:4" ht="15.6">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
     </row>
     <row r="6" spans="1:4" ht="21.6" customHeight="1">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="38" t="s">
+      <c r="C6" s="21"/>
+      <c r="D6" s="43" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21.6" customHeight="1">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="38"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="43"/>
     </row>
     <row r="8" spans="1:4" ht="21.6" customHeight="1">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
     </row>
     <row r="9" spans="1:4" ht="21.6" customHeight="1">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
     </row>
     <row r="11" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="30" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1" thickTop="1">
-      <c r="A12" s="41"/>
-      <c r="B12" s="37" t="s">
+      <c r="A12" s="37"/>
+      <c r="B12" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="39"/>
+      <c r="D12" s="35"/>
     </row>
     <row r="13" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A13" s="42"/>
-      <c r="B13" s="37" t="s">
+      <c r="A13" s="38"/>
+      <c r="B13" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="40"/>
+      <c r="D13" s="36"/>
     </row>
     <row r="14" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A14" s="42"/>
-      <c r="B14" s="37" t="s">
+      <c r="A14" s="38"/>
+      <c r="B14" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="40"/>
+      <c r="D14" s="36"/>
     </row>
     <row r="15" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A15" s="42"/>
-      <c r="B15" s="37" t="s">
+      <c r="A15" s="38"/>
+      <c r="B15" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="40"/>
+      <c r="D15" s="36"/>
     </row>
     <row r="16" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A16" s="42"/>
-      <c r="B16" s="37" t="s">
+      <c r="A16" s="38"/>
+      <c r="B16" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="40"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="36"/>
     </row>
     <row r="17" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A17" s="42"/>
-      <c r="B17" s="37" t="s">
+      <c r="A17" s="38"/>
+      <c r="B17" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="40"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="36"/>
     </row>
     <row r="18" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A18" s="42"/>
-      <c r="B18" s="37" t="s">
+      <c r="A18" s="38"/>
+      <c r="B18" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="40"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="36"/>
     </row>
     <row r="19" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A19" s="42"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="40"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="36"/>
     </row>
     <row r="20" spans="1:4" s="14" customFormat="1" ht="35.549999999999997" customHeight="1">
-      <c r="A20" s="43"/>
-      <c r="B20" s="35" t="s">
+      <c r="A20" s="39"/>
+      <c r="B20" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
     </row>
     <row r="21" spans="1:4" s="14" customFormat="1"/>
     <row r="22" spans="1:4" s="14" customFormat="1"/>
@@ -1930,7 +1999,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
@@ -1943,133 +2014,184 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="46">
         <v>5</v>
       </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="21.75" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="15.6">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
     </row>
     <row r="6" spans="1:4" ht="21.6" customHeight="1">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="44"/>
+      <c r="D6" s="43" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="21.6" customHeight="1">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="D7" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="B7" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="44"/>
+      <c r="D7" s="43"/>
     </row>
     <row r="8" spans="1:4" ht="21.6" customHeight="1">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
     </row>
     <row r="9" spans="1:4" ht="21.6" customHeight="1">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
     </row>
     <row r="11" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="53" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1" thickTop="1">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="18"/>
+      <c r="A12" s="54"/>
+      <c r="B12" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="56"/>
     </row>
     <row r="13" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="18"/>
+      <c r="A13" s="54"/>
+      <c r="B13" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="56"/>
     </row>
     <row r="14" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="18"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="56"/>
     </row>
     <row r="15" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="17" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="18"/>
-    </row>
-    <row r="18" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="18"/>
-    </row>
-    <row r="19" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="18"/>
+      <c r="A15" s="54"/>
+      <c r="B15" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="56"/>
+    </row>
+    <row r="16" spans="1:4" s="14" customFormat="1" ht="64.8" customHeight="1">
+      <c r="A16" s="54"/>
+      <c r="B16" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="56"/>
+    </row>
+    <row r="17" spans="1:4" s="14" customFormat="1" ht="101.4" customHeight="1">
+      <c r="A17" s="54"/>
+      <c r="B17" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="56"/>
+    </row>
+    <row r="18" spans="1:4" s="14" customFormat="1" ht="15.6" customHeight="1">
+      <c r="A18" s="54"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="56"/>
+    </row>
+    <row r="19" spans="1:4" s="14" customFormat="1" ht="16.2" customHeight="1">
+      <c r="A19" s="54"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="56"/>
     </row>
     <row r="20" spans="1:4" s="14" customFormat="1" ht="35.549999999999997" customHeight="1">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16" t="s">
-        <v>34</v>
-      </c>
+      <c r="A20" s="58"/>
+      <c r="B20" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
     </row>
     <row r="21" spans="1:4" s="14" customFormat="1"/>
     <row r="22" spans="1:4" s="14" customFormat="1"/>
@@ -2077,8 +2199,9 @@
     <row r="24" spans="1:4" s="14" customFormat="1"/>
     <row r="25" spans="1:4" s="14" customFormat="1"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="D6:D7"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.4" bottom="0.4" header="0" footer="0"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Added Sprints to Milestone Grading Sheet
</commit_message>
<xml_diff>
--- a/Milestone_Grading_Sheet.xlsx
+++ b/Milestone_Grading_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\traeg\Documents\CS461\404notfoundproj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11AB6767-059F-46F7-9414-D58548149DB8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96068396-65B1-43A2-A8FA-8B207AEF3A4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Milestone_1" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,15 @@
     <sheet name="Milestone_3" sheetId="3" r:id="rId3"/>
     <sheet name="Milestone_4" sheetId="4" r:id="rId4"/>
     <sheet name="Milestone_5" sheetId="5" r:id="rId5"/>
+    <sheet name="Spint_1" sheetId="6" r:id="rId6"/>
+    <sheet name="Sprint_2_Planning" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="82">
   <si>
     <t>CS 461: Software Engineering II</t>
   </si>
@@ -246,6 +248,30 @@
   </si>
   <si>
     <t>Joe - Pivotal Tracker | Descriptions - Team/Individualized</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Estimate</t>
+  </si>
+  <si>
+    <t>Owned By</t>
+  </si>
+  <si>
+    <t>2 (Planning)</t>
+  </si>
+  <si>
+    <t>Score /10 ea.</t>
+  </si>
+  <si>
+    <t>Developer</t>
   </si>
 </sst>
 </file>
@@ -655,7 +681,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -764,18 +790,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="18" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="18"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -816,6 +830,86 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="18" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="18" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1184,12 +1278,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
       <c r="A2" s="1" t="s">
@@ -1381,12 +1475,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
       <c r="A2" s="1" t="s">
@@ -1423,7 +1517,7 @@
       <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="57" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1434,7 +1528,7 @@
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="41"/>
+      <c r="D7" s="57"/>
     </row>
     <row r="8" spans="1:4" ht="21.6" customHeight="1">
       <c r="A8" s="7" t="s">
@@ -1590,12 +1684,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
       <c r="A2" s="1" t="s">
@@ -1632,7 +1726,7 @@
       <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="57" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1643,7 +1737,7 @@
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="41"/>
+      <c r="D7" s="57"/>
     </row>
     <row r="8" spans="1:4" ht="21.6" customHeight="1">
       <c r="A8" s="7" t="s">
@@ -1799,12 +1893,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
       <c r="A2" s="22" t="s">
@@ -1850,7 +1944,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="21"/>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="59" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1862,7 +1956,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="21"/>
-      <c r="D7" s="43"/>
+      <c r="D7" s="59"/>
     </row>
     <row r="8" spans="1:4" ht="21.6" customHeight="1">
       <c r="A8" s="28" t="s">
@@ -1999,8 +2093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2014,184 +2108,184 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickTop="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46">
+      <c r="B2" s="42">
         <v>5</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
     </row>
     <row r="3" spans="1:4" ht="21.75" customHeight="1">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="1:4" ht="15.6">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="1:4" ht="21.6" customHeight="1">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="43" t="s">
+      <c r="C6" s="40"/>
+      <c r="D6" s="59" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21.6" customHeight="1">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="43"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="59"/>
     </row>
     <row r="8" spans="1:4" ht="21.6" customHeight="1">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
     </row>
     <row r="9" spans="1:4" ht="21.6" customHeight="1">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
     </row>
     <row r="11" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="53" t="s">
+      <c r="D11" s="49" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1" thickTop="1">
-      <c r="A12" s="54"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="55" t="s">
+      <c r="C12" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="56"/>
+      <c r="D12" s="52"/>
     </row>
     <row r="13" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A13" s="54"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="55" t="s">
+      <c r="C13" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="56"/>
+      <c r="D13" s="52"/>
     </row>
     <row r="14" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A14" s="54"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="55" t="s">
+      <c r="C14" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="56"/>
+      <c r="D14" s="52"/>
     </row>
     <row r="15" spans="1:4" s="14" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A15" s="54"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="55" t="s">
+      <c r="C15" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="56"/>
+      <c r="D15" s="52"/>
     </row>
     <row r="16" spans="1:4" s="14" customFormat="1" ht="64.8" customHeight="1">
-      <c r="A16" s="54"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="55" t="s">
+      <c r="C16" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="56"/>
+      <c r="D16" s="52"/>
     </row>
     <row r="17" spans="1:4" s="14" customFormat="1" ht="101.4" customHeight="1">
-      <c r="A17" s="54"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="56"/>
+      <c r="D17" s="52"/>
     </row>
     <row r="18" spans="1:4" s="14" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A18" s="54"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="56"/>
+      <c r="A18" s="50"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
     </row>
     <row r="19" spans="1:4" s="14" customFormat="1" ht="16.2" customHeight="1">
-      <c r="A19" s="54"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="56"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
     </row>
     <row r="20" spans="1:4" s="14" customFormat="1" ht="35.549999999999997" customHeight="1">
-      <c r="A20" s="58"/>
-      <c r="B20" s="59" t="s">
+      <c r="A20" s="54"/>
+      <c r="B20" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
     </row>
     <row r="21" spans="1:4" s="14" customFormat="1"/>
     <row r="22" spans="1:4" s="14" customFormat="1"/>
@@ -2210,4 +2304,2330 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C4923D4-852B-44DE-9A50-D4D0F1E53EA3}">
+  <dimension ref="A1:BL17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="24.59765625" customWidth="1"/>
+    <col min="2" max="2" width="43.19921875" customWidth="1"/>
+    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="4" max="4" width="61.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:64" ht="23.4" thickBot="1">
+      <c r="A1" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="61"/>
+      <c r="X1" s="61"/>
+      <c r="Y1" s="61"/>
+      <c r="Z1" s="61"/>
+      <c r="AA1" s="61"/>
+      <c r="AB1" s="61"/>
+      <c r="AC1" s="61"/>
+      <c r="AD1" s="61"/>
+      <c r="AE1" s="61"/>
+      <c r="AF1" s="61"/>
+      <c r="AG1" s="61"/>
+      <c r="AH1" s="61"/>
+      <c r="AI1" s="61"/>
+      <c r="AJ1" s="61"/>
+      <c r="AK1" s="61"/>
+      <c r="AL1" s="61"/>
+      <c r="AM1" s="61"/>
+      <c r="AN1" s="61"/>
+      <c r="AO1" s="61"/>
+      <c r="AP1" s="61"/>
+      <c r="AQ1" s="61"/>
+      <c r="AR1" s="61"/>
+      <c r="AS1" s="61"/>
+      <c r="AT1" s="61"/>
+      <c r="AU1" s="61"/>
+      <c r="AV1" s="61"/>
+      <c r="AW1" s="61"/>
+      <c r="AX1" s="61"/>
+      <c r="AY1" s="61"/>
+      <c r="AZ1" s="61"/>
+      <c r="BA1" s="61"/>
+      <c r="BB1" s="61"/>
+      <c r="BC1" s="61"/>
+      <c r="BD1" s="61"/>
+      <c r="BE1" s="61"/>
+      <c r="BF1" s="61"/>
+      <c r="BG1" s="61"/>
+      <c r="BH1" s="61"/>
+      <c r="BI1" s="61"/>
+      <c r="BJ1" s="61"/>
+      <c r="BK1" s="61"/>
+      <c r="BL1" s="61"/>
+    </row>
+    <row r="2" spans="1:64" ht="16.2" thickTop="1">
+      <c r="A2" s="64" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="65">
+        <v>1</v>
+      </c>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="61"/>
+      <c r="W2" s="61"/>
+      <c r="X2" s="61"/>
+      <c r="Y2" s="61"/>
+      <c r="Z2" s="61"/>
+      <c r="AA2" s="61"/>
+      <c r="AB2" s="61"/>
+      <c r="AC2" s="61"/>
+      <c r="AD2" s="61"/>
+      <c r="AE2" s="61"/>
+      <c r="AF2" s="61"/>
+      <c r="AG2" s="61"/>
+      <c r="AH2" s="61"/>
+      <c r="AI2" s="61"/>
+      <c r="AJ2" s="61"/>
+      <c r="AK2" s="61"/>
+      <c r="AL2" s="61"/>
+      <c r="AM2" s="61"/>
+      <c r="AN2" s="61"/>
+      <c r="AO2" s="61"/>
+      <c r="AP2" s="61"/>
+      <c r="AQ2" s="61"/>
+      <c r="AR2" s="61"/>
+      <c r="AS2" s="61"/>
+      <c r="AT2" s="61"/>
+      <c r="AU2" s="61"/>
+      <c r="AV2" s="61"/>
+      <c r="AW2" s="61"/>
+      <c r="AX2" s="61"/>
+      <c r="AY2" s="61"/>
+      <c r="AZ2" s="61"/>
+      <c r="BA2" s="61"/>
+      <c r="BB2" s="61"/>
+      <c r="BC2" s="61"/>
+      <c r="BD2" s="61"/>
+      <c r="BE2" s="61"/>
+      <c r="BF2" s="61"/>
+      <c r="BG2" s="61"/>
+      <c r="BH2" s="61"/>
+      <c r="BI2" s="61"/>
+      <c r="BJ2" s="61"/>
+      <c r="BK2" s="61"/>
+      <c r="BL2" s="61"/>
+    </row>
+    <row r="3" spans="1:64" ht="15.6">
+      <c r="A3" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="61"/>
+      <c r="R3" s="61"/>
+      <c r="S3" s="61"/>
+      <c r="T3" s="61"/>
+      <c r="U3" s="61"/>
+      <c r="V3" s="61"/>
+      <c r="W3" s="61"/>
+      <c r="X3" s="61"/>
+      <c r="Y3" s="61"/>
+      <c r="Z3" s="61"/>
+      <c r="AA3" s="61"/>
+      <c r="AB3" s="61"/>
+      <c r="AC3" s="61"/>
+      <c r="AD3" s="61"/>
+      <c r="AE3" s="61"/>
+      <c r="AF3" s="61"/>
+      <c r="AG3" s="61"/>
+      <c r="AH3" s="61"/>
+      <c r="AI3" s="61"/>
+      <c r="AJ3" s="61"/>
+      <c r="AK3" s="61"/>
+      <c r="AL3" s="61"/>
+      <c r="AM3" s="61"/>
+      <c r="AN3" s="61"/>
+      <c r="AO3" s="61"/>
+      <c r="AP3" s="61"/>
+      <c r="AQ3" s="61"/>
+      <c r="AR3" s="61"/>
+      <c r="AS3" s="61"/>
+      <c r="AT3" s="61"/>
+      <c r="AU3" s="61"/>
+      <c r="AV3" s="61"/>
+      <c r="AW3" s="61"/>
+      <c r="AX3" s="61"/>
+      <c r="AY3" s="61"/>
+      <c r="AZ3" s="61"/>
+      <c r="BA3" s="61"/>
+      <c r="BB3" s="61"/>
+      <c r="BC3" s="61"/>
+      <c r="BD3" s="61"/>
+      <c r="BE3" s="61"/>
+      <c r="BF3" s="61"/>
+      <c r="BG3" s="61"/>
+      <c r="BH3" s="61"/>
+      <c r="BI3" s="61"/>
+      <c r="BJ3" s="61"/>
+      <c r="BK3" s="61"/>
+      <c r="BL3" s="61"/>
+    </row>
+    <row r="4" spans="1:64" ht="15.6">
+      <c r="A4" s="66" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="63" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="61"/>
+      <c r="R4" s="61"/>
+      <c r="S4" s="61"/>
+      <c r="T4" s="61"/>
+      <c r="U4" s="61"/>
+      <c r="V4" s="61"/>
+      <c r="W4" s="61"/>
+      <c r="X4" s="61"/>
+      <c r="Y4" s="61"/>
+      <c r="Z4" s="61"/>
+      <c r="AA4" s="61"/>
+      <c r="AB4" s="61"/>
+      <c r="AC4" s="61"/>
+      <c r="AD4" s="61"/>
+      <c r="AE4" s="61"/>
+      <c r="AF4" s="61"/>
+      <c r="AG4" s="61"/>
+      <c r="AH4" s="61"/>
+      <c r="AI4" s="61"/>
+      <c r="AJ4" s="61"/>
+      <c r="AK4" s="61"/>
+      <c r="AL4" s="61"/>
+      <c r="AM4" s="61"/>
+      <c r="AN4" s="61"/>
+      <c r="AO4" s="61"/>
+      <c r="AP4" s="61"/>
+      <c r="AQ4" s="61"/>
+      <c r="AR4" s="61"/>
+      <c r="AS4" s="61"/>
+      <c r="AT4" s="61"/>
+      <c r="AU4" s="61"/>
+      <c r="AV4" s="61"/>
+      <c r="AW4" s="61"/>
+      <c r="AX4" s="61"/>
+      <c r="AY4" s="61"/>
+      <c r="AZ4" s="61"/>
+      <c r="BA4" s="61"/>
+      <c r="BB4" s="61"/>
+      <c r="BC4" s="61"/>
+      <c r="BD4" s="61"/>
+      <c r="BE4" s="61"/>
+      <c r="BF4" s="61"/>
+      <c r="BG4" s="61"/>
+      <c r="BH4" s="61"/>
+      <c r="BI4" s="61"/>
+      <c r="BJ4" s="61"/>
+      <c r="BK4" s="61"/>
+      <c r="BL4" s="61"/>
+    </row>
+    <row r="5" spans="1:64" ht="30" customHeight="1">
+      <c r="A5" s="67"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="62"/>
+      <c r="Q5" s="62"/>
+      <c r="R5" s="62"/>
+      <c r="S5" s="62"/>
+      <c r="T5" s="62"/>
+      <c r="U5" s="62"/>
+      <c r="V5" s="62"/>
+      <c r="W5" s="62"/>
+      <c r="X5" s="62"/>
+      <c r="Y5" s="62"/>
+      <c r="Z5" s="62"/>
+      <c r="AA5" s="62"/>
+      <c r="AB5" s="62"/>
+      <c r="AC5" s="62"/>
+      <c r="AD5" s="62"/>
+      <c r="AE5" s="62"/>
+      <c r="AF5" s="62"/>
+      <c r="AG5" s="62"/>
+      <c r="AH5" s="62"/>
+      <c r="AI5" s="62"/>
+      <c r="AJ5" s="62"/>
+      <c r="AK5" s="62"/>
+      <c r="AL5" s="62"/>
+      <c r="AM5" s="62"/>
+      <c r="AN5" s="62"/>
+      <c r="AO5" s="62"/>
+      <c r="AP5" s="62"/>
+      <c r="AQ5" s="62"/>
+      <c r="AR5" s="62"/>
+      <c r="AS5" s="62"/>
+      <c r="AT5" s="62"/>
+      <c r="AU5" s="62"/>
+      <c r="AV5" s="62"/>
+      <c r="AW5" s="62"/>
+      <c r="AX5" s="62"/>
+      <c r="AY5" s="62"/>
+      <c r="AZ5" s="62"/>
+      <c r="BA5" s="62"/>
+      <c r="BB5" s="62"/>
+      <c r="BC5" s="62"/>
+      <c r="BD5" s="62"/>
+      <c r="BE5" s="62"/>
+      <c r="BF5" s="62"/>
+      <c r="BG5" s="62"/>
+      <c r="BH5" s="62"/>
+      <c r="BI5" s="62"/>
+      <c r="BJ5" s="62"/>
+      <c r="BK5" s="62"/>
+      <c r="BL5" s="62"/>
+    </row>
+    <row r="6" spans="1:64" ht="30" customHeight="1">
+      <c r="A6" s="67"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="62"/>
+      <c r="O6" s="62"/>
+      <c r="P6" s="62"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="62"/>
+      <c r="S6" s="62"/>
+      <c r="T6" s="62"/>
+      <c r="U6" s="62"/>
+      <c r="V6" s="62"/>
+      <c r="W6" s="62"/>
+      <c r="X6" s="62"/>
+      <c r="Y6" s="62"/>
+      <c r="Z6" s="62"/>
+      <c r="AA6" s="62"/>
+      <c r="AB6" s="62"/>
+      <c r="AC6" s="62"/>
+      <c r="AD6" s="62"/>
+      <c r="AE6" s="62"/>
+      <c r="AF6" s="62"/>
+      <c r="AG6" s="62"/>
+      <c r="AH6" s="62"/>
+      <c r="AI6" s="62"/>
+      <c r="AJ6" s="62"/>
+      <c r="AK6" s="62"/>
+      <c r="AL6" s="62"/>
+      <c r="AM6" s="62"/>
+      <c r="AN6" s="62"/>
+      <c r="AO6" s="62"/>
+      <c r="AP6" s="62"/>
+      <c r="AQ6" s="62"/>
+      <c r="AR6" s="62"/>
+      <c r="AS6" s="62"/>
+      <c r="AT6" s="62"/>
+      <c r="AU6" s="62"/>
+      <c r="AV6" s="62"/>
+      <c r="AW6" s="62"/>
+      <c r="AX6" s="62"/>
+      <c r="AY6" s="62"/>
+      <c r="AZ6" s="62"/>
+      <c r="BA6" s="62"/>
+      <c r="BB6" s="62"/>
+      <c r="BC6" s="62"/>
+      <c r="BD6" s="62"/>
+      <c r="BE6" s="62"/>
+      <c r="BF6" s="62"/>
+      <c r="BG6" s="62"/>
+      <c r="BH6" s="62"/>
+      <c r="BI6" s="62"/>
+      <c r="BJ6" s="62"/>
+      <c r="BK6" s="62"/>
+      <c r="BL6" s="62"/>
+    </row>
+    <row r="7" spans="1:64" ht="30" customHeight="1">
+      <c r="A7" s="67"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="62"/>
+      <c r="O7" s="62"/>
+      <c r="P7" s="62"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="62"/>
+      <c r="S7" s="62"/>
+      <c r="T7" s="62"/>
+      <c r="U7" s="62"/>
+      <c r="V7" s="62"/>
+      <c r="W7" s="62"/>
+      <c r="X7" s="62"/>
+      <c r="Y7" s="62"/>
+      <c r="Z7" s="62"/>
+      <c r="AA7" s="62"/>
+      <c r="AB7" s="62"/>
+      <c r="AC7" s="62"/>
+      <c r="AD7" s="62"/>
+      <c r="AE7" s="62"/>
+      <c r="AF7" s="62"/>
+      <c r="AG7" s="62"/>
+      <c r="AH7" s="62"/>
+      <c r="AI7" s="62"/>
+      <c r="AJ7" s="62"/>
+      <c r="AK7" s="62"/>
+      <c r="AL7" s="62"/>
+      <c r="AM7" s="62"/>
+      <c r="AN7" s="62"/>
+      <c r="AO7" s="62"/>
+      <c r="AP7" s="62"/>
+      <c r="AQ7" s="62"/>
+      <c r="AR7" s="62"/>
+      <c r="AS7" s="62"/>
+      <c r="AT7" s="62"/>
+      <c r="AU7" s="62"/>
+      <c r="AV7" s="62"/>
+      <c r="AW7" s="62"/>
+      <c r="AX7" s="62"/>
+      <c r="AY7" s="62"/>
+      <c r="AZ7" s="62"/>
+      <c r="BA7" s="62"/>
+      <c r="BB7" s="62"/>
+      <c r="BC7" s="62"/>
+      <c r="BD7" s="62"/>
+      <c r="BE7" s="62"/>
+      <c r="BF7" s="62"/>
+      <c r="BG7" s="62"/>
+      <c r="BH7" s="62"/>
+      <c r="BI7" s="62"/>
+      <c r="BJ7" s="62"/>
+      <c r="BK7" s="62"/>
+      <c r="BL7" s="62"/>
+    </row>
+    <row r="8" spans="1:64" ht="30" customHeight="1">
+      <c r="A8" s="67"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="62"/>
+      <c r="N8" s="62"/>
+      <c r="O8" s="62"/>
+      <c r="P8" s="62"/>
+      <c r="Q8" s="62"/>
+      <c r="R8" s="62"/>
+      <c r="S8" s="62"/>
+      <c r="T8" s="62"/>
+      <c r="U8" s="62"/>
+      <c r="V8" s="62"/>
+      <c r="W8" s="62"/>
+      <c r="X8" s="62"/>
+      <c r="Y8" s="62"/>
+      <c r="Z8" s="62"/>
+      <c r="AA8" s="62"/>
+      <c r="AB8" s="62"/>
+      <c r="AC8" s="62"/>
+      <c r="AD8" s="62"/>
+      <c r="AE8" s="62"/>
+      <c r="AF8" s="62"/>
+      <c r="AG8" s="62"/>
+      <c r="AH8" s="62"/>
+      <c r="AI8" s="62"/>
+      <c r="AJ8" s="62"/>
+      <c r="AK8" s="62"/>
+      <c r="AL8" s="62"/>
+      <c r="AM8" s="62"/>
+      <c r="AN8" s="62"/>
+      <c r="AO8" s="62"/>
+      <c r="AP8" s="62"/>
+      <c r="AQ8" s="62"/>
+      <c r="AR8" s="62"/>
+      <c r="AS8" s="62"/>
+      <c r="AT8" s="62"/>
+      <c r="AU8" s="62"/>
+      <c r="AV8" s="62"/>
+      <c r="AW8" s="62"/>
+      <c r="AX8" s="62"/>
+      <c r="AY8" s="62"/>
+      <c r="AZ8" s="62"/>
+      <c r="BA8" s="62"/>
+      <c r="BB8" s="62"/>
+      <c r="BC8" s="62"/>
+      <c r="BD8" s="62"/>
+      <c r="BE8" s="62"/>
+      <c r="BF8" s="62"/>
+      <c r="BG8" s="62"/>
+      <c r="BH8" s="62"/>
+      <c r="BI8" s="62"/>
+      <c r="BJ8" s="62"/>
+      <c r="BK8" s="62"/>
+      <c r="BL8" s="62"/>
+    </row>
+    <row r="9" spans="1:64" ht="30" customHeight="1">
+      <c r="A9" s="67"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="62"/>
+      <c r="M9" s="62"/>
+      <c r="N9" s="62"/>
+      <c r="O9" s="62"/>
+      <c r="P9" s="62"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="62"/>
+      <c r="S9" s="62"/>
+      <c r="T9" s="62"/>
+      <c r="U9" s="62"/>
+      <c r="V9" s="62"/>
+      <c r="W9" s="62"/>
+      <c r="X9" s="62"/>
+      <c r="Y9" s="62"/>
+      <c r="Z9" s="62"/>
+      <c r="AA9" s="62"/>
+      <c r="AB9" s="62"/>
+      <c r="AC9" s="62"/>
+      <c r="AD9" s="62"/>
+      <c r="AE9" s="62"/>
+      <c r="AF9" s="62"/>
+      <c r="AG9" s="62"/>
+      <c r="AH9" s="62"/>
+      <c r="AI9" s="62"/>
+      <c r="AJ9" s="62"/>
+      <c r="AK9" s="62"/>
+      <c r="AL9" s="62"/>
+      <c r="AM9" s="62"/>
+      <c r="AN9" s="62"/>
+      <c r="AO9" s="62"/>
+      <c r="AP9" s="62"/>
+      <c r="AQ9" s="62"/>
+      <c r="AR9" s="62"/>
+      <c r="AS9" s="62"/>
+      <c r="AT9" s="62"/>
+      <c r="AU9" s="62"/>
+      <c r="AV9" s="62"/>
+      <c r="AW9" s="62"/>
+      <c r="AX9" s="62"/>
+      <c r="AY9" s="62"/>
+      <c r="AZ9" s="62"/>
+      <c r="BA9" s="62"/>
+      <c r="BB9" s="62"/>
+      <c r="BC9" s="62"/>
+      <c r="BD9" s="62"/>
+      <c r="BE9" s="62"/>
+      <c r="BF9" s="62"/>
+      <c r="BG9" s="62"/>
+      <c r="BH9" s="62"/>
+      <c r="BI9" s="62"/>
+      <c r="BJ9" s="62"/>
+      <c r="BK9" s="62"/>
+      <c r="BL9" s="62"/>
+    </row>
+    <row r="10" spans="1:64" ht="30" customHeight="1">
+      <c r="A10" s="67"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="62"/>
+      <c r="O10" s="62"/>
+      <c r="P10" s="62"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="62"/>
+      <c r="T10" s="62"/>
+      <c r="U10" s="62"/>
+      <c r="V10" s="62"/>
+      <c r="W10" s="62"/>
+      <c r="X10" s="62"/>
+      <c r="Y10" s="62"/>
+      <c r="Z10" s="62"/>
+      <c r="AA10" s="62"/>
+      <c r="AB10" s="62"/>
+      <c r="AC10" s="62"/>
+      <c r="AD10" s="62"/>
+      <c r="AE10" s="62"/>
+      <c r="AF10" s="62"/>
+      <c r="AG10" s="62"/>
+      <c r="AH10" s="62"/>
+      <c r="AI10" s="62"/>
+      <c r="AJ10" s="62"/>
+      <c r="AK10" s="62"/>
+      <c r="AL10" s="62"/>
+      <c r="AM10" s="62"/>
+      <c r="AN10" s="62"/>
+      <c r="AO10" s="62"/>
+      <c r="AP10" s="62"/>
+      <c r="AQ10" s="62"/>
+      <c r="AR10" s="62"/>
+      <c r="AS10" s="62"/>
+      <c r="AT10" s="62"/>
+      <c r="AU10" s="62"/>
+      <c r="AV10" s="62"/>
+      <c r="AW10" s="62"/>
+      <c r="AX10" s="62"/>
+      <c r="AY10" s="62"/>
+      <c r="AZ10" s="62"/>
+      <c r="BA10" s="62"/>
+      <c r="BB10" s="62"/>
+      <c r="BC10" s="62"/>
+      <c r="BD10" s="62"/>
+      <c r="BE10" s="62"/>
+      <c r="BF10" s="62"/>
+      <c r="BG10" s="62"/>
+      <c r="BH10" s="62"/>
+      <c r="BI10" s="62"/>
+      <c r="BJ10" s="62"/>
+      <c r="BK10" s="62"/>
+      <c r="BL10" s="62"/>
+    </row>
+    <row r="11" spans="1:64" ht="30" customHeight="1">
+      <c r="A11" s="67"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="62"/>
+      <c r="N11" s="62"/>
+      <c r="O11" s="62"/>
+      <c r="P11" s="62"/>
+      <c r="Q11" s="62"/>
+      <c r="R11" s="62"/>
+      <c r="S11" s="62"/>
+      <c r="T11" s="62"/>
+      <c r="U11" s="62"/>
+      <c r="V11" s="62"/>
+      <c r="W11" s="62"/>
+      <c r="X11" s="62"/>
+      <c r="Y11" s="62"/>
+      <c r="Z11" s="62"/>
+      <c r="AA11" s="62"/>
+      <c r="AB11" s="62"/>
+      <c r="AC11" s="62"/>
+      <c r="AD11" s="62"/>
+      <c r="AE11" s="62"/>
+      <c r="AF11" s="62"/>
+      <c r="AG11" s="62"/>
+      <c r="AH11" s="62"/>
+      <c r="AI11" s="62"/>
+      <c r="AJ11" s="62"/>
+      <c r="AK11" s="62"/>
+      <c r="AL11" s="62"/>
+      <c r="AM11" s="62"/>
+      <c r="AN11" s="62"/>
+      <c r="AO11" s="62"/>
+      <c r="AP11" s="62"/>
+      <c r="AQ11" s="62"/>
+      <c r="AR11" s="62"/>
+      <c r="AS11" s="62"/>
+      <c r="AT11" s="62"/>
+      <c r="AU11" s="62"/>
+      <c r="AV11" s="62"/>
+      <c r="AW11" s="62"/>
+      <c r="AX11" s="62"/>
+      <c r="AY11" s="62"/>
+      <c r="AZ11" s="62"/>
+      <c r="BA11" s="62"/>
+      <c r="BB11" s="62"/>
+      <c r="BC11" s="62"/>
+      <c r="BD11" s="62"/>
+      <c r="BE11" s="62"/>
+      <c r="BF11" s="62"/>
+      <c r="BG11" s="62"/>
+      <c r="BH11" s="62"/>
+      <c r="BI11" s="62"/>
+      <c r="BJ11" s="62"/>
+      <c r="BK11" s="62"/>
+      <c r="BL11" s="62"/>
+    </row>
+    <row r="12" spans="1:64" ht="30" customHeight="1">
+      <c r="A12" s="67"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="62"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="62"/>
+      <c r="N12" s="62"/>
+      <c r="O12" s="62"/>
+      <c r="P12" s="62"/>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="62"/>
+      <c r="S12" s="62"/>
+      <c r="T12" s="62"/>
+      <c r="U12" s="62"/>
+      <c r="V12" s="62"/>
+      <c r="W12" s="62"/>
+      <c r="X12" s="62"/>
+      <c r="Y12" s="62"/>
+      <c r="Z12" s="62"/>
+      <c r="AA12" s="62"/>
+      <c r="AB12" s="62"/>
+      <c r="AC12" s="62"/>
+      <c r="AD12" s="62"/>
+      <c r="AE12" s="62"/>
+      <c r="AF12" s="62"/>
+      <c r="AG12" s="62"/>
+      <c r="AH12" s="62"/>
+      <c r="AI12" s="62"/>
+      <c r="AJ12" s="62"/>
+      <c r="AK12" s="62"/>
+      <c r="AL12" s="62"/>
+      <c r="AM12" s="62"/>
+      <c r="AN12" s="62"/>
+      <c r="AO12" s="62"/>
+      <c r="AP12" s="62"/>
+      <c r="AQ12" s="62"/>
+      <c r="AR12" s="62"/>
+      <c r="AS12" s="62"/>
+      <c r="AT12" s="62"/>
+      <c r="AU12" s="62"/>
+      <c r="AV12" s="62"/>
+      <c r="AW12" s="62"/>
+      <c r="AX12" s="62"/>
+      <c r="AY12" s="62"/>
+      <c r="AZ12" s="62"/>
+      <c r="BA12" s="62"/>
+      <c r="BB12" s="62"/>
+      <c r="BC12" s="62"/>
+      <c r="BD12" s="62"/>
+      <c r="BE12" s="62"/>
+      <c r="BF12" s="62"/>
+      <c r="BG12" s="62"/>
+      <c r="BH12" s="62"/>
+      <c r="BI12" s="62"/>
+      <c r="BJ12" s="62"/>
+      <c r="BK12" s="62"/>
+      <c r="BL12" s="62"/>
+    </row>
+    <row r="13" spans="1:64" ht="30" customHeight="1">
+      <c r="A13" s="67"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="62"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="62"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="62"/>
+      <c r="S13" s="62"/>
+      <c r="T13" s="62"/>
+      <c r="U13" s="62"/>
+      <c r="V13" s="62"/>
+      <c r="W13" s="62"/>
+      <c r="X13" s="62"/>
+      <c r="Y13" s="62"/>
+      <c r="Z13" s="62"/>
+      <c r="AA13" s="62"/>
+      <c r="AB13" s="62"/>
+      <c r="AC13" s="62"/>
+      <c r="AD13" s="62"/>
+      <c r="AE13" s="62"/>
+      <c r="AF13" s="62"/>
+      <c r="AG13" s="62"/>
+      <c r="AH13" s="62"/>
+      <c r="AI13" s="62"/>
+      <c r="AJ13" s="62"/>
+      <c r="AK13" s="62"/>
+      <c r="AL13" s="62"/>
+      <c r="AM13" s="62"/>
+      <c r="AN13" s="62"/>
+      <c r="AO13" s="62"/>
+      <c r="AP13" s="62"/>
+      <c r="AQ13" s="62"/>
+      <c r="AR13" s="62"/>
+      <c r="AS13" s="62"/>
+      <c r="AT13" s="62"/>
+      <c r="AU13" s="62"/>
+      <c r="AV13" s="62"/>
+      <c r="AW13" s="62"/>
+      <c r="AX13" s="62"/>
+      <c r="AY13" s="62"/>
+      <c r="AZ13" s="62"/>
+      <c r="BA13" s="62"/>
+      <c r="BB13" s="62"/>
+      <c r="BC13" s="62"/>
+      <c r="BD13" s="62"/>
+      <c r="BE13" s="62"/>
+      <c r="BF13" s="62"/>
+      <c r="BG13" s="62"/>
+      <c r="BH13" s="62"/>
+      <c r="BI13" s="62"/>
+      <c r="BJ13" s="62"/>
+      <c r="BK13" s="62"/>
+      <c r="BL13" s="62"/>
+    </row>
+    <row r="14" spans="1:64" ht="30" customHeight="1">
+      <c r="A14" s="67"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="62"/>
+      <c r="N14" s="62"/>
+      <c r="O14" s="62"/>
+      <c r="P14" s="62"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="62"/>
+      <c r="S14" s="62"/>
+      <c r="T14" s="62"/>
+      <c r="U14" s="62"/>
+      <c r="V14" s="62"/>
+      <c r="W14" s="62"/>
+      <c r="X14" s="62"/>
+      <c r="Y14" s="62"/>
+      <c r="Z14" s="62"/>
+      <c r="AA14" s="62"/>
+      <c r="AB14" s="62"/>
+      <c r="AC14" s="62"/>
+      <c r="AD14" s="62"/>
+      <c r="AE14" s="62"/>
+      <c r="AF14" s="62"/>
+      <c r="AG14" s="62"/>
+      <c r="AH14" s="62"/>
+      <c r="AI14" s="62"/>
+      <c r="AJ14" s="62"/>
+      <c r="AK14" s="62"/>
+      <c r="AL14" s="62"/>
+      <c r="AM14" s="62"/>
+      <c r="AN14" s="62"/>
+      <c r="AO14" s="62"/>
+      <c r="AP14" s="62"/>
+      <c r="AQ14" s="62"/>
+      <c r="AR14" s="62"/>
+      <c r="AS14" s="62"/>
+      <c r="AT14" s="62"/>
+      <c r="AU14" s="62"/>
+      <c r="AV14" s="62"/>
+      <c r="AW14" s="62"/>
+      <c r="AX14" s="62"/>
+      <c r="AY14" s="62"/>
+      <c r="AZ14" s="62"/>
+      <c r="BA14" s="62"/>
+      <c r="BB14" s="62"/>
+      <c r="BC14" s="62"/>
+      <c r="BD14" s="62"/>
+      <c r="BE14" s="62"/>
+      <c r="BF14" s="62"/>
+      <c r="BG14" s="62"/>
+      <c r="BH14" s="62"/>
+      <c r="BI14" s="62"/>
+      <c r="BJ14" s="62"/>
+      <c r="BK14" s="62"/>
+      <c r="BL14" s="62"/>
+    </row>
+    <row r="15" spans="1:64">
+      <c r="A15" s="70"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="62"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="62"/>
+      <c r="M15" s="62"/>
+      <c r="N15" s="62"/>
+      <c r="O15" s="62"/>
+      <c r="P15" s="62"/>
+      <c r="Q15" s="62"/>
+      <c r="R15" s="62"/>
+      <c r="S15" s="62"/>
+      <c r="T15" s="62"/>
+      <c r="U15" s="62"/>
+      <c r="V15" s="62"/>
+      <c r="W15" s="62"/>
+      <c r="X15" s="62"/>
+      <c r="Y15" s="62"/>
+      <c r="Z15" s="62"/>
+      <c r="AA15" s="62"/>
+      <c r="AB15" s="62"/>
+      <c r="AC15" s="62"/>
+      <c r="AD15" s="62"/>
+      <c r="AE15" s="62"/>
+      <c r="AF15" s="62"/>
+      <c r="AG15" s="62"/>
+      <c r="AH15" s="62"/>
+      <c r="AI15" s="62"/>
+      <c r="AJ15" s="62"/>
+      <c r="AK15" s="62"/>
+      <c r="AL15" s="62"/>
+      <c r="AM15" s="62"/>
+      <c r="AN15" s="62"/>
+      <c r="AO15" s="62"/>
+      <c r="AP15" s="62"/>
+      <c r="AQ15" s="62"/>
+      <c r="AR15" s="62"/>
+      <c r="AS15" s="62"/>
+      <c r="AT15" s="62"/>
+      <c r="AU15" s="62"/>
+      <c r="AV15" s="62"/>
+      <c r="AW15" s="62"/>
+      <c r="AX15" s="62"/>
+      <c r="AY15" s="62"/>
+      <c r="AZ15" s="62"/>
+      <c r="BA15" s="62"/>
+      <c r="BB15" s="62"/>
+      <c r="BC15" s="62"/>
+      <c r="BD15" s="62"/>
+      <c r="BE15" s="62"/>
+      <c r="BF15" s="62"/>
+      <c r="BG15" s="62"/>
+      <c r="BH15" s="62"/>
+      <c r="BI15" s="62"/>
+      <c r="BJ15" s="62"/>
+      <c r="BK15" s="62"/>
+      <c r="BL15" s="62"/>
+    </row>
+    <row r="16" spans="1:64">
+      <c r="A16" s="70"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="62"/>
+      <c r="K16" s="62"/>
+      <c r="L16" s="62"/>
+      <c r="M16" s="62"/>
+      <c r="N16" s="62"/>
+      <c r="O16" s="62"/>
+      <c r="P16" s="62"/>
+      <c r="Q16" s="62"/>
+      <c r="R16" s="62"/>
+      <c r="S16" s="62"/>
+      <c r="T16" s="62"/>
+      <c r="U16" s="62"/>
+      <c r="V16" s="62"/>
+      <c r="W16" s="62"/>
+      <c r="X16" s="62"/>
+      <c r="Y16" s="62"/>
+      <c r="Z16" s="62"/>
+      <c r="AA16" s="62"/>
+      <c r="AB16" s="62"/>
+      <c r="AC16" s="62"/>
+      <c r="AD16" s="62"/>
+      <c r="AE16" s="62"/>
+      <c r="AF16" s="62"/>
+      <c r="AG16" s="62"/>
+      <c r="AH16" s="62"/>
+      <c r="AI16" s="62"/>
+      <c r="AJ16" s="62"/>
+      <c r="AK16" s="62"/>
+      <c r="AL16" s="62"/>
+      <c r="AM16" s="62"/>
+      <c r="AN16" s="62"/>
+      <c r="AO16" s="62"/>
+      <c r="AP16" s="62"/>
+      <c r="AQ16" s="62"/>
+      <c r="AR16" s="62"/>
+      <c r="AS16" s="62"/>
+      <c r="AT16" s="62"/>
+      <c r="AU16" s="62"/>
+      <c r="AV16" s="62"/>
+      <c r="AW16" s="62"/>
+      <c r="AX16" s="62"/>
+      <c r="AY16" s="62"/>
+      <c r="AZ16" s="62"/>
+      <c r="BA16" s="62"/>
+      <c r="BB16" s="62"/>
+      <c r="BC16" s="62"/>
+      <c r="BD16" s="62"/>
+      <c r="BE16" s="62"/>
+      <c r="BF16" s="62"/>
+      <c r="BG16" s="62"/>
+      <c r="BH16" s="62"/>
+      <c r="BI16" s="62"/>
+      <c r="BJ16" s="62"/>
+      <c r="BK16" s="62"/>
+      <c r="BL16" s="62"/>
+    </row>
+    <row r="17" spans="1:64">
+      <c r="A17" s="70"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="62"/>
+      <c r="O17" s="62"/>
+      <c r="P17" s="62"/>
+      <c r="Q17" s="62"/>
+      <c r="R17" s="62"/>
+      <c r="S17" s="62"/>
+      <c r="T17" s="62"/>
+      <c r="U17" s="62"/>
+      <c r="V17" s="62"/>
+      <c r="W17" s="62"/>
+      <c r="X17" s="62"/>
+      <c r="Y17" s="62"/>
+      <c r="Z17" s="62"/>
+      <c r="AA17" s="62"/>
+      <c r="AB17" s="62"/>
+      <c r="AC17" s="62"/>
+      <c r="AD17" s="62"/>
+      <c r="AE17" s="62"/>
+      <c r="AF17" s="62"/>
+      <c r="AG17" s="62"/>
+      <c r="AH17" s="62"/>
+      <c r="AI17" s="62"/>
+      <c r="AJ17" s="62"/>
+      <c r="AK17" s="62"/>
+      <c r="AL17" s="62"/>
+      <c r="AM17" s="62"/>
+      <c r="AN17" s="62"/>
+      <c r="AO17" s="62"/>
+      <c r="AP17" s="62"/>
+      <c r="AQ17" s="62"/>
+      <c r="AR17" s="62"/>
+      <c r="AS17" s="62"/>
+      <c r="AT17" s="62"/>
+      <c r="AU17" s="62"/>
+      <c r="AV17" s="62"/>
+      <c r="AW17" s="62"/>
+      <c r="AX17" s="62"/>
+      <c r="AY17" s="62"/>
+      <c r="AZ17" s="62"/>
+      <c r="BA17" s="62"/>
+      <c r="BB17" s="62"/>
+      <c r="BC17" s="62"/>
+      <c r="BD17" s="62"/>
+      <c r="BE17" s="62"/>
+      <c r="BF17" s="62"/>
+      <c r="BG17" s="62"/>
+      <c r="BH17" s="62"/>
+      <c r="BI17" s="62"/>
+      <c r="BJ17" s="62"/>
+      <c r="BK17" s="62"/>
+      <c r="BL17" s="62"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A7587A-86AE-48BC-A95D-C54B44C1364E}">
+  <dimension ref="A1:BL17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
+    <col min="3" max="3" width="58.796875" customWidth="1"/>
+    <col min="4" max="4" width="26.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:64" ht="23.4" thickBot="1">
+      <c r="A1" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
+      <c r="AA1" s="73"/>
+      <c r="AB1" s="73"/>
+      <c r="AC1" s="73"/>
+      <c r="AD1" s="73"/>
+      <c r="AE1" s="73"/>
+      <c r="AF1" s="73"/>
+      <c r="AG1" s="73"/>
+      <c r="AH1" s="73"/>
+      <c r="AI1" s="73"/>
+      <c r="AJ1" s="73"/>
+      <c r="AK1" s="73"/>
+      <c r="AL1" s="73"/>
+      <c r="AM1" s="73"/>
+      <c r="AN1" s="73"/>
+      <c r="AO1" s="73"/>
+      <c r="AP1" s="73"/>
+      <c r="AQ1" s="73"/>
+      <c r="AR1" s="73"/>
+      <c r="AS1" s="73"/>
+      <c r="AT1" s="73"/>
+      <c r="AU1" s="73"/>
+      <c r="AV1" s="73"/>
+      <c r="AW1" s="73"/>
+      <c r="AX1" s="73"/>
+      <c r="AY1" s="73"/>
+      <c r="AZ1" s="73"/>
+      <c r="BA1" s="73"/>
+      <c r="BB1" s="73"/>
+      <c r="BC1" s="73"/>
+      <c r="BD1" s="73"/>
+      <c r="BE1" s="73"/>
+      <c r="BF1" s="73"/>
+      <c r="BG1" s="73"/>
+      <c r="BH1" s="73"/>
+      <c r="BI1" s="73"/>
+      <c r="BJ1" s="73"/>
+      <c r="BK1" s="73"/>
+      <c r="BL1" s="73"/>
+    </row>
+    <row r="2" spans="1:64" ht="16.2" thickTop="1">
+      <c r="A2" s="75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="72" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="73"/>
+      <c r="V2" s="73"/>
+      <c r="W2" s="73"/>
+      <c r="X2" s="73"/>
+      <c r="Y2" s="73"/>
+      <c r="Z2" s="73"/>
+      <c r="AA2" s="73"/>
+      <c r="AB2" s="73"/>
+      <c r="AC2" s="73"/>
+      <c r="AD2" s="73"/>
+      <c r="AE2" s="73"/>
+      <c r="AF2" s="73"/>
+      <c r="AG2" s="73"/>
+      <c r="AH2" s="73"/>
+      <c r="AI2" s="73"/>
+      <c r="AJ2" s="73"/>
+      <c r="AK2" s="73"/>
+      <c r="AL2" s="73"/>
+      <c r="AM2" s="73"/>
+      <c r="AN2" s="73"/>
+      <c r="AO2" s="73"/>
+      <c r="AP2" s="73"/>
+      <c r="AQ2" s="73"/>
+      <c r="AR2" s="73"/>
+      <c r="AS2" s="73"/>
+      <c r="AT2" s="73"/>
+      <c r="AU2" s="73"/>
+      <c r="AV2" s="73"/>
+      <c r="AW2" s="73"/>
+      <c r="AX2" s="73"/>
+      <c r="AY2" s="73"/>
+      <c r="AZ2" s="73"/>
+      <c r="BA2" s="73"/>
+      <c r="BB2" s="73"/>
+      <c r="BC2" s="73"/>
+      <c r="BD2" s="73"/>
+      <c r="BE2" s="73"/>
+      <c r="BF2" s="73"/>
+      <c r="BG2" s="73"/>
+      <c r="BH2" s="73"/>
+      <c r="BI2" s="73"/>
+      <c r="BJ2" s="73"/>
+      <c r="BK2" s="73"/>
+      <c r="BL2" s="73"/>
+    </row>
+    <row r="3" spans="1:64" ht="15.6">
+      <c r="A3" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="73"/>
+      <c r="T3" s="73"/>
+      <c r="U3" s="73"/>
+      <c r="V3" s="73"/>
+      <c r="W3" s="73"/>
+      <c r="X3" s="73"/>
+      <c r="Y3" s="73"/>
+      <c r="Z3" s="73"/>
+      <c r="AA3" s="73"/>
+      <c r="AB3" s="73"/>
+      <c r="AC3" s="73"/>
+      <c r="AD3" s="73"/>
+      <c r="AE3" s="73"/>
+      <c r="AF3" s="73"/>
+      <c r="AG3" s="73"/>
+      <c r="AH3" s="73"/>
+      <c r="AI3" s="73"/>
+      <c r="AJ3" s="73"/>
+      <c r="AK3" s="73"/>
+      <c r="AL3" s="73"/>
+      <c r="AM3" s="73"/>
+      <c r="AN3" s="73"/>
+      <c r="AO3" s="73"/>
+      <c r="AP3" s="73"/>
+      <c r="AQ3" s="73"/>
+      <c r="AR3" s="73"/>
+      <c r="AS3" s="73"/>
+      <c r="AT3" s="73"/>
+      <c r="AU3" s="73"/>
+      <c r="AV3" s="73"/>
+      <c r="AW3" s="73"/>
+      <c r="AX3" s="73"/>
+      <c r="AY3" s="73"/>
+      <c r="AZ3" s="73"/>
+      <c r="BA3" s="73"/>
+      <c r="BB3" s="73"/>
+      <c r="BC3" s="73"/>
+      <c r="BD3" s="73"/>
+      <c r="BE3" s="73"/>
+      <c r="BF3" s="73"/>
+      <c r="BG3" s="73"/>
+      <c r="BH3" s="73"/>
+      <c r="BI3" s="73"/>
+      <c r="BJ3" s="73"/>
+      <c r="BK3" s="73"/>
+      <c r="BL3" s="73"/>
+    </row>
+    <row r="4" spans="1:64" ht="15.6">
+      <c r="A4" s="76" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="82" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="73"/>
+      <c r="R4" s="73"/>
+      <c r="S4" s="73"/>
+      <c r="T4" s="73"/>
+      <c r="U4" s="73"/>
+      <c r="V4" s="73"/>
+      <c r="W4" s="73"/>
+      <c r="X4" s="73"/>
+      <c r="Y4" s="73"/>
+      <c r="Z4" s="73"/>
+      <c r="AA4" s="73"/>
+      <c r="AB4" s="73"/>
+      <c r="AC4" s="73"/>
+      <c r="AD4" s="73"/>
+      <c r="AE4" s="73"/>
+      <c r="AF4" s="73"/>
+      <c r="AG4" s="73"/>
+      <c r="AH4" s="73"/>
+      <c r="AI4" s="73"/>
+      <c r="AJ4" s="73"/>
+      <c r="AK4" s="73"/>
+      <c r="AL4" s="73"/>
+      <c r="AM4" s="73"/>
+      <c r="AN4" s="73"/>
+      <c r="AO4" s="73"/>
+      <c r="AP4" s="73"/>
+      <c r="AQ4" s="73"/>
+      <c r="AR4" s="73"/>
+      <c r="AS4" s="73"/>
+      <c r="AT4" s="73"/>
+      <c r="AU4" s="73"/>
+      <c r="AV4" s="73"/>
+      <c r="AW4" s="73"/>
+      <c r="AX4" s="73"/>
+      <c r="AY4" s="73"/>
+      <c r="AZ4" s="73"/>
+      <c r="BA4" s="73"/>
+      <c r="BB4" s="73"/>
+      <c r="BC4" s="73"/>
+      <c r="BD4" s="73"/>
+      <c r="BE4" s="73"/>
+      <c r="BF4" s="73"/>
+      <c r="BG4" s="73"/>
+      <c r="BH4" s="73"/>
+      <c r="BI4" s="73"/>
+      <c r="BJ4" s="73"/>
+      <c r="BK4" s="73"/>
+      <c r="BL4" s="73"/>
+    </row>
+    <row r="5" spans="1:64" ht="30" customHeight="1">
+      <c r="A5" s="77"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="74"/>
+      <c r="Q5" s="74"/>
+      <c r="R5" s="74"/>
+      <c r="S5" s="74"/>
+      <c r="T5" s="74"/>
+      <c r="U5" s="74"/>
+      <c r="V5" s="74"/>
+      <c r="W5" s="74"/>
+      <c r="X5" s="74"/>
+      <c r="Y5" s="74"/>
+      <c r="Z5" s="74"/>
+      <c r="AA5" s="74"/>
+      <c r="AB5" s="74"/>
+      <c r="AC5" s="74"/>
+      <c r="AD5" s="74"/>
+      <c r="AE5" s="74"/>
+      <c r="AF5" s="74"/>
+      <c r="AG5" s="74"/>
+      <c r="AH5" s="74"/>
+      <c r="AI5" s="74"/>
+      <c r="AJ5" s="74"/>
+      <c r="AK5" s="74"/>
+      <c r="AL5" s="74"/>
+      <c r="AM5" s="74"/>
+      <c r="AN5" s="74"/>
+      <c r="AO5" s="74"/>
+      <c r="AP5" s="74"/>
+      <c r="AQ5" s="74"/>
+      <c r="AR5" s="74"/>
+      <c r="AS5" s="74"/>
+      <c r="AT5" s="74"/>
+      <c r="AU5" s="74"/>
+      <c r="AV5" s="74"/>
+      <c r="AW5" s="74"/>
+      <c r="AX5" s="74"/>
+      <c r="AY5" s="74"/>
+      <c r="AZ5" s="74"/>
+      <c r="BA5" s="74"/>
+      <c r="BB5" s="74"/>
+      <c r="BC5" s="74"/>
+      <c r="BD5" s="74"/>
+      <c r="BE5" s="74"/>
+      <c r="BF5" s="74"/>
+      <c r="BG5" s="74"/>
+      <c r="BH5" s="74"/>
+      <c r="BI5" s="74"/>
+      <c r="BJ5" s="74"/>
+      <c r="BK5" s="74"/>
+      <c r="BL5" s="74"/>
+    </row>
+    <row r="6" spans="1:64" ht="30" customHeight="1">
+      <c r="A6" s="77"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="74"/>
+      <c r="M6" s="74"/>
+      <c r="N6" s="74"/>
+      <c r="O6" s="74"/>
+      <c r="P6" s="74"/>
+      <c r="Q6" s="74"/>
+      <c r="R6" s="74"/>
+      <c r="S6" s="74"/>
+      <c r="T6" s="74"/>
+      <c r="U6" s="74"/>
+      <c r="V6" s="74"/>
+      <c r="W6" s="74"/>
+      <c r="X6" s="74"/>
+      <c r="Y6" s="74"/>
+      <c r="Z6" s="74"/>
+      <c r="AA6" s="74"/>
+      <c r="AB6" s="74"/>
+      <c r="AC6" s="74"/>
+      <c r="AD6" s="74"/>
+      <c r="AE6" s="74"/>
+      <c r="AF6" s="74"/>
+      <c r="AG6" s="74"/>
+      <c r="AH6" s="74"/>
+      <c r="AI6" s="74"/>
+      <c r="AJ6" s="74"/>
+      <c r="AK6" s="74"/>
+      <c r="AL6" s="74"/>
+      <c r="AM6" s="74"/>
+      <c r="AN6" s="74"/>
+      <c r="AO6" s="74"/>
+      <c r="AP6" s="74"/>
+      <c r="AQ6" s="74"/>
+      <c r="AR6" s="74"/>
+      <c r="AS6" s="74"/>
+      <c r="AT6" s="74"/>
+      <c r="AU6" s="74"/>
+      <c r="AV6" s="74"/>
+      <c r="AW6" s="74"/>
+      <c r="AX6" s="74"/>
+      <c r="AY6" s="74"/>
+      <c r="AZ6" s="74"/>
+      <c r="BA6" s="74"/>
+      <c r="BB6" s="74"/>
+      <c r="BC6" s="74"/>
+      <c r="BD6" s="74"/>
+      <c r="BE6" s="74"/>
+      <c r="BF6" s="74"/>
+      <c r="BG6" s="74"/>
+      <c r="BH6" s="74"/>
+      <c r="BI6" s="74"/>
+      <c r="BJ6" s="74"/>
+      <c r="BK6" s="74"/>
+      <c r="BL6" s="74"/>
+    </row>
+    <row r="7" spans="1:64" ht="30" customHeight="1">
+      <c r="A7" s="77"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="74"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="74"/>
+      <c r="V7" s="74"/>
+      <c r="W7" s="74"/>
+      <c r="X7" s="74"/>
+      <c r="Y7" s="74"/>
+      <c r="Z7" s="74"/>
+      <c r="AA7" s="74"/>
+      <c r="AB7" s="74"/>
+      <c r="AC7" s="74"/>
+      <c r="AD7" s="74"/>
+      <c r="AE7" s="74"/>
+      <c r="AF7" s="74"/>
+      <c r="AG7" s="74"/>
+      <c r="AH7" s="74"/>
+      <c r="AI7" s="74"/>
+      <c r="AJ7" s="74"/>
+      <c r="AK7" s="74"/>
+      <c r="AL7" s="74"/>
+      <c r="AM7" s="74"/>
+      <c r="AN7" s="74"/>
+      <c r="AO7" s="74"/>
+      <c r="AP7" s="74"/>
+      <c r="AQ7" s="74"/>
+      <c r="AR7" s="74"/>
+      <c r="AS7" s="74"/>
+      <c r="AT7" s="74"/>
+      <c r="AU7" s="74"/>
+      <c r="AV7" s="74"/>
+      <c r="AW7" s="74"/>
+      <c r="AX7" s="74"/>
+      <c r="AY7" s="74"/>
+      <c r="AZ7" s="74"/>
+      <c r="BA7" s="74"/>
+      <c r="BB7" s="74"/>
+      <c r="BC7" s="74"/>
+      <c r="BD7" s="74"/>
+      <c r="BE7" s="74"/>
+      <c r="BF7" s="74"/>
+      <c r="BG7" s="74"/>
+      <c r="BH7" s="74"/>
+      <c r="BI7" s="74"/>
+      <c r="BJ7" s="74"/>
+      <c r="BK7" s="74"/>
+      <c r="BL7" s="74"/>
+    </row>
+    <row r="8" spans="1:64" ht="30" customHeight="1">
+      <c r="A8" s="77"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="74"/>
+      <c r="Q8" s="74"/>
+      <c r="R8" s="74"/>
+      <c r="S8" s="74"/>
+      <c r="T8" s="74"/>
+      <c r="U8" s="74"/>
+      <c r="V8" s="74"/>
+      <c r="W8" s="74"/>
+      <c r="X8" s="74"/>
+      <c r="Y8" s="74"/>
+      <c r="Z8" s="74"/>
+      <c r="AA8" s="74"/>
+      <c r="AB8" s="74"/>
+      <c r="AC8" s="74"/>
+      <c r="AD8" s="74"/>
+      <c r="AE8" s="74"/>
+      <c r="AF8" s="74"/>
+      <c r="AG8" s="74"/>
+      <c r="AH8" s="74"/>
+      <c r="AI8" s="74"/>
+      <c r="AJ8" s="74"/>
+      <c r="AK8" s="74"/>
+      <c r="AL8" s="74"/>
+      <c r="AM8" s="74"/>
+      <c r="AN8" s="74"/>
+      <c r="AO8" s="74"/>
+      <c r="AP8" s="74"/>
+      <c r="AQ8" s="74"/>
+      <c r="AR8" s="74"/>
+      <c r="AS8" s="74"/>
+      <c r="AT8" s="74"/>
+      <c r="AU8" s="74"/>
+      <c r="AV8" s="74"/>
+      <c r="AW8" s="74"/>
+      <c r="AX8" s="74"/>
+      <c r="AY8" s="74"/>
+      <c r="AZ8" s="74"/>
+      <c r="BA8" s="74"/>
+      <c r="BB8" s="74"/>
+      <c r="BC8" s="74"/>
+      <c r="BD8" s="74"/>
+      <c r="BE8" s="74"/>
+      <c r="BF8" s="74"/>
+      <c r="BG8" s="74"/>
+      <c r="BH8" s="74"/>
+      <c r="BI8" s="74"/>
+      <c r="BJ8" s="74"/>
+      <c r="BK8" s="74"/>
+      <c r="BL8" s="74"/>
+    </row>
+    <row r="9" spans="1:64">
+      <c r="A9" s="73"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="74"/>
+      <c r="N9" s="74"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74"/>
+      <c r="Q9" s="74"/>
+      <c r="R9" s="74"/>
+      <c r="S9" s="74"/>
+      <c r="T9" s="74"/>
+      <c r="U9" s="74"/>
+      <c r="V9" s="74"/>
+      <c r="W9" s="74"/>
+      <c r="X9" s="74"/>
+      <c r="Y9" s="74"/>
+      <c r="Z9" s="74"/>
+      <c r="AA9" s="74"/>
+      <c r="AB9" s="74"/>
+      <c r="AC9" s="74"/>
+      <c r="AD9" s="74"/>
+      <c r="AE9" s="74"/>
+      <c r="AF9" s="74"/>
+      <c r="AG9" s="74"/>
+      <c r="AH9" s="74"/>
+      <c r="AI9" s="74"/>
+      <c r="AJ9" s="74"/>
+      <c r="AK9" s="74"/>
+      <c r="AL9" s="74"/>
+      <c r="AM9" s="74"/>
+      <c r="AN9" s="74"/>
+      <c r="AO9" s="74"/>
+      <c r="AP9" s="74"/>
+      <c r="AQ9" s="74"/>
+      <c r="AR9" s="74"/>
+      <c r="AS9" s="74"/>
+      <c r="AT9" s="74"/>
+      <c r="AU9" s="74"/>
+      <c r="AV9" s="74"/>
+      <c r="AW9" s="74"/>
+      <c r="AX9" s="74"/>
+      <c r="AY9" s="74"/>
+      <c r="AZ9" s="74"/>
+      <c r="BA9" s="74"/>
+      <c r="BB9" s="74"/>
+      <c r="BC9" s="74"/>
+      <c r="BD9" s="74"/>
+      <c r="BE9" s="74"/>
+      <c r="BF9" s="74"/>
+      <c r="BG9" s="74"/>
+      <c r="BH9" s="74"/>
+      <c r="BI9" s="74"/>
+      <c r="BJ9" s="74"/>
+      <c r="BK9" s="74"/>
+      <c r="BL9" s="74"/>
+    </row>
+    <row r="10" spans="1:64">
+      <c r="A10" s="73"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="74"/>
+      <c r="K10" s="74"/>
+      <c r="L10" s="74"/>
+      <c r="M10" s="74"/>
+      <c r="N10" s="74"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
+      <c r="R10" s="74"/>
+      <c r="S10" s="74"/>
+      <c r="T10" s="74"/>
+      <c r="U10" s="74"/>
+      <c r="V10" s="74"/>
+      <c r="W10" s="74"/>
+      <c r="X10" s="74"/>
+      <c r="Y10" s="74"/>
+      <c r="Z10" s="74"/>
+      <c r="AA10" s="74"/>
+      <c r="AB10" s="74"/>
+      <c r="AC10" s="74"/>
+      <c r="AD10" s="74"/>
+      <c r="AE10" s="74"/>
+      <c r="AF10" s="74"/>
+      <c r="AG10" s="74"/>
+      <c r="AH10" s="74"/>
+      <c r="AI10" s="74"/>
+      <c r="AJ10" s="74"/>
+      <c r="AK10" s="74"/>
+      <c r="AL10" s="74"/>
+      <c r="AM10" s="74"/>
+      <c r="AN10" s="74"/>
+      <c r="AO10" s="74"/>
+      <c r="AP10" s="74"/>
+      <c r="AQ10" s="74"/>
+      <c r="AR10" s="74"/>
+      <c r="AS10" s="74"/>
+      <c r="AT10" s="74"/>
+      <c r="AU10" s="74"/>
+      <c r="AV10" s="74"/>
+      <c r="AW10" s="74"/>
+      <c r="AX10" s="74"/>
+      <c r="AY10" s="74"/>
+      <c r="AZ10" s="74"/>
+      <c r="BA10" s="74"/>
+      <c r="BB10" s="74"/>
+      <c r="BC10" s="74"/>
+      <c r="BD10" s="74"/>
+      <c r="BE10" s="74"/>
+      <c r="BF10" s="74"/>
+      <c r="BG10" s="74"/>
+      <c r="BH10" s="74"/>
+      <c r="BI10" s="74"/>
+      <c r="BJ10" s="74"/>
+      <c r="BK10" s="74"/>
+      <c r="BL10" s="74"/>
+    </row>
+    <row r="11" spans="1:64">
+      <c r="A11" s="73"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="74"/>
+      <c r="L11" s="74"/>
+      <c r="M11" s="74"/>
+      <c r="N11" s="74"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
+      <c r="R11" s="74"/>
+      <c r="S11" s="74"/>
+      <c r="T11" s="74"/>
+      <c r="U11" s="74"/>
+      <c r="V11" s="74"/>
+      <c r="W11" s="74"/>
+      <c r="X11" s="74"/>
+      <c r="Y11" s="74"/>
+      <c r="Z11" s="74"/>
+      <c r="AA11" s="74"/>
+      <c r="AB11" s="74"/>
+      <c r="AC11" s="74"/>
+      <c r="AD11" s="74"/>
+      <c r="AE11" s="74"/>
+      <c r="AF11" s="74"/>
+      <c r="AG11" s="74"/>
+      <c r="AH11" s="74"/>
+      <c r="AI11" s="74"/>
+      <c r="AJ11" s="74"/>
+      <c r="AK11" s="74"/>
+      <c r="AL11" s="74"/>
+      <c r="AM11" s="74"/>
+      <c r="AN11" s="74"/>
+      <c r="AO11" s="74"/>
+      <c r="AP11" s="74"/>
+      <c r="AQ11" s="74"/>
+      <c r="AR11" s="74"/>
+      <c r="AS11" s="74"/>
+      <c r="AT11" s="74"/>
+      <c r="AU11" s="74"/>
+      <c r="AV11" s="74"/>
+      <c r="AW11" s="74"/>
+      <c r="AX11" s="74"/>
+      <c r="AY11" s="74"/>
+      <c r="AZ11" s="74"/>
+      <c r="BA11" s="74"/>
+      <c r="BB11" s="74"/>
+      <c r="BC11" s="74"/>
+      <c r="BD11" s="74"/>
+      <c r="BE11" s="74"/>
+      <c r="BF11" s="74"/>
+      <c r="BG11" s="74"/>
+      <c r="BH11" s="74"/>
+      <c r="BI11" s="74"/>
+      <c r="BJ11" s="74"/>
+      <c r="BK11" s="74"/>
+      <c r="BL11" s="74"/>
+    </row>
+    <row r="12" spans="1:64">
+      <c r="A12" s="73"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="74"/>
+      <c r="J12" s="74"/>
+      <c r="K12" s="74"/>
+      <c r="L12" s="74"/>
+      <c r="M12" s="74"/>
+      <c r="N12" s="74"/>
+      <c r="O12" s="74"/>
+      <c r="P12" s="74"/>
+      <c r="Q12" s="74"/>
+      <c r="R12" s="74"/>
+      <c r="S12" s="74"/>
+      <c r="T12" s="74"/>
+      <c r="U12" s="74"/>
+      <c r="V12" s="74"/>
+      <c r="W12" s="74"/>
+      <c r="X12" s="74"/>
+      <c r="Y12" s="74"/>
+      <c r="Z12" s="74"/>
+      <c r="AA12" s="74"/>
+      <c r="AB12" s="74"/>
+      <c r="AC12" s="74"/>
+      <c r="AD12" s="74"/>
+      <c r="AE12" s="74"/>
+      <c r="AF12" s="74"/>
+      <c r="AG12" s="74"/>
+      <c r="AH12" s="74"/>
+      <c r="AI12" s="74"/>
+      <c r="AJ12" s="74"/>
+      <c r="AK12" s="74"/>
+      <c r="AL12" s="74"/>
+      <c r="AM12" s="74"/>
+      <c r="AN12" s="74"/>
+      <c r="AO12" s="74"/>
+      <c r="AP12" s="74"/>
+      <c r="AQ12" s="74"/>
+      <c r="AR12" s="74"/>
+      <c r="AS12" s="74"/>
+      <c r="AT12" s="74"/>
+      <c r="AU12" s="74"/>
+      <c r="AV12" s="74"/>
+      <c r="AW12" s="74"/>
+      <c r="AX12" s="74"/>
+      <c r="AY12" s="74"/>
+      <c r="AZ12" s="74"/>
+      <c r="BA12" s="74"/>
+      <c r="BB12" s="74"/>
+      <c r="BC12" s="74"/>
+      <c r="BD12" s="74"/>
+      <c r="BE12" s="74"/>
+      <c r="BF12" s="74"/>
+      <c r="BG12" s="74"/>
+      <c r="BH12" s="74"/>
+      <c r="BI12" s="74"/>
+      <c r="BJ12" s="74"/>
+      <c r="BK12" s="74"/>
+      <c r="BL12" s="74"/>
+    </row>
+    <row r="13" spans="1:64">
+      <c r="A13" s="73"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="74"/>
+      <c r="L13" s="74"/>
+      <c r="M13" s="74"/>
+      <c r="N13" s="74"/>
+      <c r="O13" s="74"/>
+      <c r="P13" s="74"/>
+      <c r="Q13" s="74"/>
+      <c r="R13" s="74"/>
+      <c r="S13" s="74"/>
+      <c r="T13" s="74"/>
+      <c r="U13" s="74"/>
+      <c r="V13" s="74"/>
+      <c r="W13" s="74"/>
+      <c r="X13" s="74"/>
+      <c r="Y13" s="74"/>
+      <c r="Z13" s="74"/>
+      <c r="AA13" s="74"/>
+      <c r="AB13" s="74"/>
+      <c r="AC13" s="74"/>
+      <c r="AD13" s="74"/>
+      <c r="AE13" s="74"/>
+      <c r="AF13" s="74"/>
+      <c r="AG13" s="74"/>
+      <c r="AH13" s="74"/>
+      <c r="AI13" s="74"/>
+      <c r="AJ13" s="74"/>
+      <c r="AK13" s="74"/>
+      <c r="AL13" s="74"/>
+      <c r="AM13" s="74"/>
+      <c r="AN13" s="74"/>
+      <c r="AO13" s="74"/>
+      <c r="AP13" s="74"/>
+      <c r="AQ13" s="74"/>
+      <c r="AR13" s="74"/>
+      <c r="AS13" s="74"/>
+      <c r="AT13" s="74"/>
+      <c r="AU13" s="74"/>
+      <c r="AV13" s="74"/>
+      <c r="AW13" s="74"/>
+      <c r="AX13" s="74"/>
+      <c r="AY13" s="74"/>
+      <c r="AZ13" s="74"/>
+      <c r="BA13" s="74"/>
+      <c r="BB13" s="74"/>
+      <c r="BC13" s="74"/>
+      <c r="BD13" s="74"/>
+      <c r="BE13" s="74"/>
+      <c r="BF13" s="74"/>
+      <c r="BG13" s="74"/>
+      <c r="BH13" s="74"/>
+      <c r="BI13" s="74"/>
+      <c r="BJ13" s="74"/>
+      <c r="BK13" s="74"/>
+      <c r="BL13" s="74"/>
+    </row>
+    <row r="14" spans="1:64">
+      <c r="A14" s="73"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="74"/>
+      <c r="J14" s="74"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="74"/>
+      <c r="M14" s="74"/>
+      <c r="N14" s="74"/>
+      <c r="O14" s="74"/>
+      <c r="P14" s="74"/>
+      <c r="Q14" s="74"/>
+      <c r="R14" s="74"/>
+      <c r="S14" s="74"/>
+      <c r="T14" s="74"/>
+      <c r="U14" s="74"/>
+      <c r="V14" s="74"/>
+      <c r="W14" s="74"/>
+      <c r="X14" s="74"/>
+      <c r="Y14" s="74"/>
+      <c r="Z14" s="74"/>
+      <c r="AA14" s="74"/>
+      <c r="AB14" s="74"/>
+      <c r="AC14" s="74"/>
+      <c r="AD14" s="74"/>
+      <c r="AE14" s="74"/>
+      <c r="AF14" s="74"/>
+      <c r="AG14" s="74"/>
+      <c r="AH14" s="74"/>
+      <c r="AI14" s="74"/>
+      <c r="AJ14" s="74"/>
+      <c r="AK14" s="74"/>
+      <c r="AL14" s="74"/>
+      <c r="AM14" s="74"/>
+      <c r="AN14" s="74"/>
+      <c r="AO14" s="74"/>
+      <c r="AP14" s="74"/>
+      <c r="AQ14" s="74"/>
+      <c r="AR14" s="74"/>
+      <c r="AS14" s="74"/>
+      <c r="AT14" s="74"/>
+      <c r="AU14" s="74"/>
+      <c r="AV14" s="74"/>
+      <c r="AW14" s="74"/>
+      <c r="AX14" s="74"/>
+      <c r="AY14" s="74"/>
+      <c r="AZ14" s="74"/>
+      <c r="BA14" s="74"/>
+      <c r="BB14" s="74"/>
+      <c r="BC14" s="74"/>
+      <c r="BD14" s="74"/>
+      <c r="BE14" s="74"/>
+      <c r="BF14" s="74"/>
+      <c r="BG14" s="74"/>
+      <c r="BH14" s="74"/>
+      <c r="BI14" s="74"/>
+      <c r="BJ14" s="74"/>
+      <c r="BK14" s="74"/>
+      <c r="BL14" s="74"/>
+    </row>
+    <row r="15" spans="1:64">
+      <c r="A15" s="80"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="74"/>
+      <c r="L15" s="74"/>
+      <c r="M15" s="74"/>
+      <c r="N15" s="74"/>
+      <c r="O15" s="74"/>
+      <c r="P15" s="74"/>
+      <c r="Q15" s="74"/>
+      <c r="R15" s="74"/>
+      <c r="S15" s="74"/>
+      <c r="T15" s="74"/>
+      <c r="U15" s="74"/>
+      <c r="V15" s="74"/>
+      <c r="W15" s="74"/>
+      <c r="X15" s="74"/>
+      <c r="Y15" s="74"/>
+      <c r="Z15" s="74"/>
+      <c r="AA15" s="74"/>
+      <c r="AB15" s="74"/>
+      <c r="AC15" s="74"/>
+      <c r="AD15" s="74"/>
+      <c r="AE15" s="74"/>
+      <c r="AF15" s="74"/>
+      <c r="AG15" s="74"/>
+      <c r="AH15" s="74"/>
+      <c r="AI15" s="74"/>
+      <c r="AJ15" s="74"/>
+      <c r="AK15" s="74"/>
+      <c r="AL15" s="74"/>
+      <c r="AM15" s="74"/>
+      <c r="AN15" s="74"/>
+      <c r="AO15" s="74"/>
+      <c r="AP15" s="74"/>
+      <c r="AQ15" s="74"/>
+      <c r="AR15" s="74"/>
+      <c r="AS15" s="74"/>
+      <c r="AT15" s="74"/>
+      <c r="AU15" s="74"/>
+      <c r="AV15" s="74"/>
+      <c r="AW15" s="74"/>
+      <c r="AX15" s="74"/>
+      <c r="AY15" s="74"/>
+      <c r="AZ15" s="74"/>
+      <c r="BA15" s="74"/>
+      <c r="BB15" s="74"/>
+      <c r="BC15" s="74"/>
+      <c r="BD15" s="74"/>
+      <c r="BE15" s="74"/>
+      <c r="BF15" s="74"/>
+      <c r="BG15" s="74"/>
+      <c r="BH15" s="74"/>
+      <c r="BI15" s="74"/>
+      <c r="BJ15" s="74"/>
+      <c r="BK15" s="74"/>
+      <c r="BL15" s="74"/>
+    </row>
+    <row r="16" spans="1:64">
+      <c r="A16" s="80"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="74"/>
+      <c r="L16" s="74"/>
+      <c r="M16" s="74"/>
+      <c r="N16" s="74"/>
+      <c r="O16" s="74"/>
+      <c r="P16" s="74"/>
+      <c r="Q16" s="74"/>
+      <c r="R16" s="74"/>
+      <c r="S16" s="74"/>
+      <c r="T16" s="74"/>
+      <c r="U16" s="74"/>
+      <c r="V16" s="74"/>
+      <c r="W16" s="74"/>
+      <c r="X16" s="74"/>
+      <c r="Y16" s="74"/>
+      <c r="Z16" s="74"/>
+      <c r="AA16" s="74"/>
+      <c r="AB16" s="74"/>
+      <c r="AC16" s="74"/>
+      <c r="AD16" s="74"/>
+      <c r="AE16" s="74"/>
+      <c r="AF16" s="74"/>
+      <c r="AG16" s="74"/>
+      <c r="AH16" s="74"/>
+      <c r="AI16" s="74"/>
+      <c r="AJ16" s="74"/>
+      <c r="AK16" s="74"/>
+      <c r="AL16" s="74"/>
+      <c r="AM16" s="74"/>
+      <c r="AN16" s="74"/>
+      <c r="AO16" s="74"/>
+      <c r="AP16" s="74"/>
+      <c r="AQ16" s="74"/>
+      <c r="AR16" s="74"/>
+      <c r="AS16" s="74"/>
+      <c r="AT16" s="74"/>
+      <c r="AU16" s="74"/>
+      <c r="AV16" s="74"/>
+      <c r="AW16" s="74"/>
+      <c r="AX16" s="74"/>
+      <c r="AY16" s="74"/>
+      <c r="AZ16" s="74"/>
+      <c r="BA16" s="74"/>
+      <c r="BB16" s="74"/>
+      <c r="BC16" s="74"/>
+      <c r="BD16" s="74"/>
+      <c r="BE16" s="74"/>
+      <c r="BF16" s="74"/>
+      <c r="BG16" s="74"/>
+      <c r="BH16" s="74"/>
+      <c r="BI16" s="74"/>
+      <c r="BJ16" s="74"/>
+      <c r="BK16" s="74"/>
+      <c r="BL16" s="74"/>
+    </row>
+    <row r="17" spans="1:64">
+      <c r="A17" s="80"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="74"/>
+      <c r="K17" s="74"/>
+      <c r="L17" s="74"/>
+      <c r="M17" s="74"/>
+      <c r="N17" s="74"/>
+      <c r="O17" s="74"/>
+      <c r="P17" s="74"/>
+      <c r="Q17" s="74"/>
+      <c r="R17" s="74"/>
+      <c r="S17" s="74"/>
+      <c r="T17" s="74"/>
+      <c r="U17" s="74"/>
+      <c r="V17" s="74"/>
+      <c r="W17" s="74"/>
+      <c r="X17" s="74"/>
+      <c r="Y17" s="74"/>
+      <c r="Z17" s="74"/>
+      <c r="AA17" s="74"/>
+      <c r="AB17" s="74"/>
+      <c r="AC17" s="74"/>
+      <c r="AD17" s="74"/>
+      <c r="AE17" s="74"/>
+      <c r="AF17" s="74"/>
+      <c r="AG17" s="74"/>
+      <c r="AH17" s="74"/>
+      <c r="AI17" s="74"/>
+      <c r="AJ17" s="74"/>
+      <c r="AK17" s="74"/>
+      <c r="AL17" s="74"/>
+      <c r="AM17" s="74"/>
+      <c r="AN17" s="74"/>
+      <c r="AO17" s="74"/>
+      <c r="AP17" s="74"/>
+      <c r="AQ17" s="74"/>
+      <c r="AR17" s="74"/>
+      <c r="AS17" s="74"/>
+      <c r="AT17" s="74"/>
+      <c r="AU17" s="74"/>
+      <c r="AV17" s="74"/>
+      <c r="AW17" s="74"/>
+      <c r="AX17" s="74"/>
+      <c r="AY17" s="74"/>
+      <c r="AZ17" s="74"/>
+      <c r="BA17" s="74"/>
+      <c r="BB17" s="74"/>
+      <c r="BC17" s="74"/>
+      <c r="BD17" s="74"/>
+      <c r="BE17" s="74"/>
+      <c r="BF17" s="74"/>
+      <c r="BG17" s="74"/>
+      <c r="BH17" s="74"/>
+      <c r="BI17" s="74"/>
+      <c r="BJ17" s="74"/>
+      <c r="BK17" s="74"/>
+      <c r="BL17" s="74"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>